<commit_message>
LUTs causing strange bug
</commit_message>
<xml_diff>
--- a/Assets/Docs/LookupTables.xlsx
+++ b/Assets/Docs/LookupTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Lookup table:</t>
   </si>
@@ -161,46 +161,52 @@
     <t>significant bits</t>
   </si>
   <si>
-    <t>(a &lt;&lt; 23) &amp; 0b100000000000000000000000</t>
-  </si>
-  <si>
     <t>(b &lt;&lt; 19) &amp; 0b11110000000000000000000</t>
   </si>
   <si>
     <t>final</t>
   </si>
   <si>
-    <t>(b &lt;&lt; 19) &amp; 0b011110000000000000000000</t>
-  </si>
-  <si>
-    <t>(c &lt;&lt; 15) &amp; 0b000001000000000000000000</t>
-  </si>
-  <si>
-    <t>(d &lt;&lt; 13) &amp; 0b000000100000000000000000</t>
-  </si>
-  <si>
-    <t>(d &lt;&lt; 11) &amp; 0b000000000000100000000000</t>
-  </si>
-  <si>
-    <t>(e &lt;&lt; 05) &amp; 0b000000000001000000000000</t>
-  </si>
-  <si>
-    <t>(e &lt;&lt; 03) &amp; 0b000000000000000001000000</t>
-  </si>
-  <si>
-    <t>(f &lt;&lt; 01) &amp; 0b000000000000000000100000</t>
-  </si>
-  <si>
-    <t>(g &gt;&gt; 03) &amp; 0b000000000000000000011110</t>
-  </si>
-  <si>
-    <t>(h &gt;&gt; 07) &amp; 0b000000000000000000000001</t>
-  </si>
-  <si>
-    <t>(x &lt;&lt; 09) &amp; 0b000000011110000000000000</t>
-  </si>
-  <si>
-    <t>(x &lt;&lt; 07) &amp; 0b000000000000011110000000</t>
+    <t>(a &lt;&lt; 23) &amp; 8388608</t>
+  </si>
+  <si>
+    <t>(b &lt;&lt; 19) &amp; 7864320</t>
+  </si>
+  <si>
+    <t>(c &lt;&lt; 15) &amp; 262144</t>
+  </si>
+  <si>
+    <t>(d &lt;&lt; 13) &amp; 131072</t>
+  </si>
+  <si>
+    <t>(d &lt;&lt; 11) &amp; 2048</t>
+  </si>
+  <si>
+    <t>(e &lt;&lt; 05) &amp; 4096</t>
+  </si>
+  <si>
+    <t>(e &lt;&lt; 03) &amp; 64</t>
+  </si>
+  <si>
+    <t>(f &lt;&lt; 01) &amp; 32</t>
+  </si>
+  <si>
+    <t>(g &gt;&gt; 03) &amp; 30</t>
+  </si>
+  <si>
+    <t>(h &gt;&gt; 07) &amp; 1</t>
+  </si>
+  <si>
+    <t>(x &lt;&lt; 09) &amp; 122880</t>
+  </si>
+  <si>
+    <t>(x &lt;&lt; 07) &amp; 1920</t>
+  </si>
+  <si>
+    <t>Get local bit:</t>
+  </si>
+  <si>
+    <t>(chunkData &gt;&gt; (7 - x - 4 * y)) &amp; 1</t>
   </si>
 </sst>
 </file>
@@ -656,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -889,21 +895,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,6 +914,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -934,7 +937,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -947,6 +953,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,8 +998,8 @@
       <xdr:rowOff>12112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>130967</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>5267</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>12112</xdr:rowOff>
     </xdr:to>
@@ -996,7 +1011,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="757892" y="10513425"/>
-          <a:ext cx="4123669" cy="3500437"/>
+          <a:ext cx="4248000" cy="3500437"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1046,7 +1061,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((a &lt;&lt; 23) &amp; 0b100000000000000000000000) +</a:t>
+            <a:t>((a &lt;&lt; 23) &amp; 8388608) +</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1060,7 +1075,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((b &lt;&lt; 19) &amp; 0b011110000000000000000000) +</a:t>
+            <a:t>((b &lt;&lt; 19) &amp; 7864320) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1077,7 +1092,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((c &lt;&lt; 15) &amp; 0b000001000000000000000000) +</a:t>
+            <a:t>((c &lt;&lt; 15) &amp; 262144) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1094,7 +1109,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((d &lt;&lt; 13) &amp; 0b000000100000000000000000) +</a:t>
+            <a:t>((d &lt;&lt; 13) &amp; 131072) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1111,7 +1126,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((d &lt;&lt; 11) &amp; 0b000000000000100000000000) +</a:t>
+            <a:t>((d &lt;&lt; 11) &amp; 2048) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1128,7 +1143,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((e &lt;&lt; 05) &amp; 0b000000000001000000000000) +</a:t>
+            <a:t>((e &lt;&lt; 05) &amp; 4096) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1145,7 +1160,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((e &lt;&lt; 03) &amp; 0b000000000000000001000000) +</a:t>
+            <a:t>((e &lt;&lt; 03) &amp; 64) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1162,7 +1177,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((f &lt;&lt; 01) &amp; 0b000000000000000000100000) +</a:t>
+            <a:t>((f &lt;&lt; 01) &amp; 32) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1179,7 +1194,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((g &gt;&gt; 03) &amp; 0b000000000000000000011110) +</a:t>
+            <a:t>((g &gt;&gt; 03) &amp; 30) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1196,7 +1211,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((h &gt;&gt; 07) &amp; 0b000000000000000000000001) +</a:t>
+            <a:t>((h &gt;&gt; 07) &amp; 1) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1213,7 +1228,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((x &lt;&lt; 09) &amp; 0b000000011110000000000000) +</a:t>
+            <a:t>((x &lt;&lt; 09) &amp; 122880) +</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1230,7 +1245,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>((x &lt;&lt; 07) &amp; 0b000000000000011110000000)</a:t>
+            <a:t>((x &lt;&lt; 07) &amp; 1920);</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -1508,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AT41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AE53" sqref="AE53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27:AI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1566,28 +1581,28 @@
       <c r="O5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AI5" s="87" t="s">
+      <c r="AI5" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="AJ5" s="87" t="s">
+      <c r="AJ5" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="AK5" s="87" t="s">
+      <c r="AK5" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="AL5" s="87" t="s">
+      <c r="AL5" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="87" t="s">
+      <c r="AM5" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="AN5" s="87" t="s">
+      <c r="AN5" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="AO5" s="87" t="s">
+      <c r="AO5" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="AP5" s="87" t="s">
+      <c r="AP5" s="86" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1630,14 +1645,14 @@
       </c>
       <c r="AF6" s="52"/>
       <c r="AG6" s="44"/>
-      <c r="AI6" s="88"/>
-      <c r="AJ6" s="88"/>
-      <c r="AK6" s="88"/>
-      <c r="AL6" s="88"/>
-      <c r="AM6" s="88"/>
-      <c r="AN6" s="88"/>
-      <c r="AO6" s="88"/>
-      <c r="AP6" s="88"/>
+      <c r="AI6" s="87"/>
+      <c r="AJ6" s="87"/>
+      <c r="AK6" s="87"/>
+      <c r="AL6" s="87"/>
+      <c r="AM6" s="87"/>
+      <c r="AN6" s="87"/>
+      <c r="AO6" s="87"/>
+      <c r="AP6" s="87"/>
     </row>
     <row r="7" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
@@ -1663,10 +1678,10 @@
       </c>
       <c r="N7" s="44"/>
       <c r="O7" s="44"/>
-      <c r="R7" s="91" t="s">
+      <c r="R7" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="91"/>
+      <c r="S7" s="90"/>
       <c r="AB7" s="49">
         <v>0</v>
       </c>
@@ -1733,8 +1748,8 @@
       <c r="J8" s="7"/>
       <c r="N8" s="45"/>
       <c r="O8" s="45"/>
-      <c r="R8" s="92"/>
-      <c r="S8" s="92"/>
+      <c r="R8" s="91"/>
+      <c r="S8" s="91"/>
     </row>
     <row r="9" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
@@ -1772,6 +1787,9 @@
       </c>
       <c r="W9" s="73"/>
       <c r="X9" s="18"/>
+      <c r="AB9" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M10" s="19"/>
@@ -1798,6 +1816,9 @@
       <c r="V10" s="74"/>
       <c r="W10" s="75"/>
       <c r="X10" s="22"/>
+      <c r="AB10" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
@@ -1912,15 +1933,15 @@
       <c r="X14" s="22"/>
     </row>
     <row r="15" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R15" s="89" t="s">
+      <c r="R15" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="S15" s="89"/>
+      <c r="S15" s="88"/>
       <c r="AA15" s="8"/>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R16" s="90"/>
-      <c r="S16" s="90"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="89"/>
       <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2078,19 +2099,19 @@
       <c r="T20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="AA20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22" s="81" t="s">
+      <c r="O22" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
-      <c r="R22" s="82"/>
+      <c r="P22" s="81"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="79"/>
     </row>
     <row r="23" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D23" s="65">
@@ -2117,54 +2138,54 @@
       <c r="K23" s="65">
         <v>0</v>
       </c>
-      <c r="M23" s="81" t="s">
+      <c r="M23" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="N23" s="82"/>
-      <c r="O23" s="81" t="s">
+      <c r="N23" s="79"/>
+      <c r="O23" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="81" t="s">
+      <c r="P23" s="79"/>
+      <c r="Q23" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="82"/>
-      <c r="S23" s="81" t="s">
+      <c r="R23" s="79"/>
+      <c r="S23" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="T23" s="82"/>
-      <c r="U23" s="81" t="s">
+      <c r="T23" s="79"/>
+      <c r="U23" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="83"/>
-      <c r="W23" s="83"/>
-      <c r="X23" s="82"/>
-      <c r="Y23" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z23" s="83"/>
-      <c r="AA23" s="83"/>
-      <c r="AB23" s="83"/>
-      <c r="AC23" s="83"/>
-      <c r="AD23" s="83"/>
-      <c r="AE23" s="83"/>
-      <c r="AF23" s="83"/>
-      <c r="AG23" s="83"/>
-      <c r="AH23" s="83"/>
-      <c r="AI23" s="82"/>
-      <c r="AJ23" s="81" t="s">
+      <c r="V23" s="81"/>
+      <c r="W23" s="81"/>
+      <c r="X23" s="79"/>
+      <c r="Y23" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z23" s="81"/>
+      <c r="AA23" s="81"/>
+      <c r="AB23" s="81"/>
+      <c r="AC23" s="81"/>
+      <c r="AD23" s="81"/>
+      <c r="AE23" s="81"/>
+      <c r="AF23" s="81"/>
+      <c r="AG23" s="81"/>
+      <c r="AH23" s="81"/>
+      <c r="AI23" s="79"/>
+      <c r="AJ23" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="AK23" s="83"/>
-      <c r="AL23" s="83"/>
-      <c r="AM23" s="83"/>
-      <c r="AN23" s="83"/>
-      <c r="AO23" s="83"/>
-      <c r="AP23" s="83"/>
-      <c r="AQ23" s="83"/>
-      <c r="AR23" s="83"/>
-      <c r="AS23" s="83"/>
-      <c r="AT23" s="82"/>
+      <c r="AK23" s="81"/>
+      <c r="AL23" s="81"/>
+      <c r="AM23" s="81"/>
+      <c r="AN23" s="81"/>
+      <c r="AO23" s="81"/>
+      <c r="AP23" s="81"/>
+      <c r="AQ23" s="81"/>
+      <c r="AR23" s="81"/>
+      <c r="AS23" s="81"/>
+      <c r="AT23" s="79"/>
     </row>
     <row r="24" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -2197,39 +2218,39 @@
         <v>23</v>
       </c>
       <c r="T24" s="67"/>
-      <c r="U24" s="84">
+      <c r="U24" s="82">
         <v>1</v>
       </c>
-      <c r="V24" s="85"/>
-      <c r="W24" s="85"/>
-      <c r="X24" s="86"/>
-      <c r="Y24" s="78" t="str">
-        <f>CONCATENATE("(", B24, " &lt;&lt; ", TEXT(S24, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q24) * (POWER(2, U24) - 1), 2, 24))</f>
-        <v>(a &lt;&lt; 23) &amp; 0b100000000000000000000000</v>
-      </c>
-      <c r="Z24" s="79"/>
-      <c r="AA24" s="79"/>
-      <c r="AB24" s="79"/>
-      <c r="AC24" s="79"/>
-      <c r="AD24" s="79"/>
-      <c r="AE24" s="79"/>
-      <c r="AF24" s="79"/>
-      <c r="AG24" s="79"/>
-      <c r="AH24" s="79"/>
-      <c r="AI24" s="94"/>
-      <c r="AJ24" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK24" s="85"/>
-      <c r="AL24" s="85"/>
-      <c r="AM24" s="85"/>
-      <c r="AN24" s="85"/>
-      <c r="AO24" s="85"/>
-      <c r="AP24" s="85"/>
-      <c r="AQ24" s="85"/>
-      <c r="AR24" s="85"/>
-      <c r="AS24" s="85"/>
-      <c r="AT24" s="86"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
+      <c r="X24" s="84"/>
+      <c r="Y24" s="98" t="str">
+        <f>CONCATENATE("(", B24, " &lt;&lt; ", TEXT(S24, "00"), ") &amp; ", POWER(2, Q24) * (POWER(2, U24) - 1),)</f>
+        <v>(a &lt;&lt; 23) &amp; 8388608</v>
+      </c>
+      <c r="Z24" s="99"/>
+      <c r="AA24" s="99"/>
+      <c r="AB24" s="99"/>
+      <c r="AC24" s="99"/>
+      <c r="AD24" s="99"/>
+      <c r="AE24" s="99"/>
+      <c r="AF24" s="99"/>
+      <c r="AG24" s="99"/>
+      <c r="AH24" s="99"/>
+      <c r="AI24" s="100"/>
+      <c r="AJ24" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK24" s="83"/>
+      <c r="AL24" s="83"/>
+      <c r="AM24" s="83"/>
+      <c r="AN24" s="83"/>
+      <c r="AO24" s="83"/>
+      <c r="AP24" s="83"/>
+      <c r="AQ24" s="83"/>
+      <c r="AR24" s="83"/>
+      <c r="AS24" s="83"/>
+      <c r="AT24" s="84"/>
     </row>
     <row r="25" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M25" s="76"/>
@@ -2244,16 +2265,16 @@
       <c r="V25" s="80"/>
       <c r="W25" s="80"/>
       <c r="X25" s="67"/>
-      <c r="Y25" s="78"/>
-      <c r="Z25" s="79"/>
-      <c r="AA25" s="79"/>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="79"/>
-      <c r="AD25" s="79"/>
-      <c r="AE25" s="79"/>
-      <c r="AF25" s="79"/>
-      <c r="AG25" s="79"/>
-      <c r="AH25" s="79"/>
+      <c r="Y25" s="92"/>
+      <c r="Z25" s="93"/>
+      <c r="AA25" s="93"/>
+      <c r="AB25" s="93"/>
+      <c r="AC25" s="93"/>
+      <c r="AD25" s="93"/>
+      <c r="AE25" s="93"/>
+      <c r="AF25" s="93"/>
+      <c r="AG25" s="93"/>
+      <c r="AH25" s="93"/>
       <c r="AI25" s="94"/>
       <c r="AJ25" s="66"/>
       <c r="AK25" s="80"/>
@@ -2310,19 +2331,19 @@
       <c r="V26" s="80"/>
       <c r="W26" s="80"/>
       <c r="X26" s="67"/>
-      <c r="Y26" s="78" t="str">
-        <f>CONCATENATE("(", B26, " &lt;&lt; ", TEXT(S26, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q26) * (POWER(2, U26) - 1), 2, 24))</f>
-        <v>(b &lt;&lt; 19) &amp; 0b011110000000000000000000</v>
-      </c>
-      <c r="Z26" s="79"/>
-      <c r="AA26" s="79"/>
-      <c r="AB26" s="79"/>
-      <c r="AC26" s="79"/>
-      <c r="AD26" s="79"/>
-      <c r="AE26" s="79"/>
-      <c r="AF26" s="79"/>
-      <c r="AG26" s="79"/>
-      <c r="AH26" s="79"/>
+      <c r="Y26" s="92" t="str">
+        <f>CONCATENATE("(", B26, " &lt;&lt; ", TEXT(S26, "00"), ") &amp; ", POWER(2, Q26) * (POWER(2, U26) - 1),)</f>
+        <v>(b &lt;&lt; 19) &amp; 7864320</v>
+      </c>
+      <c r="Z26" s="93"/>
+      <c r="AA26" s="93"/>
+      <c r="AB26" s="93"/>
+      <c r="AC26" s="93"/>
+      <c r="AD26" s="93"/>
+      <c r="AE26" s="93"/>
+      <c r="AF26" s="93"/>
+      <c r="AG26" s="93"/>
+      <c r="AH26" s="93"/>
       <c r="AI26" s="94"/>
       <c r="AJ26" s="66" t="s">
         <v>48</v>
@@ -2351,16 +2372,16 @@
       <c r="V27" s="80"/>
       <c r="W27" s="80"/>
       <c r="X27" s="67"/>
-      <c r="Y27" s="78"/>
-      <c r="Z27" s="79"/>
-      <c r="AA27" s="79"/>
-      <c r="AB27" s="79"/>
-      <c r="AC27" s="79"/>
-      <c r="AD27" s="79"/>
-      <c r="AE27" s="79"/>
-      <c r="AF27" s="79"/>
-      <c r="AG27" s="79"/>
-      <c r="AH27" s="79"/>
+      <c r="Y27" s="92"/>
+      <c r="Z27" s="93"/>
+      <c r="AA27" s="93"/>
+      <c r="AB27" s="93"/>
+      <c r="AC27" s="93"/>
+      <c r="AD27" s="93"/>
+      <c r="AE27" s="93"/>
+      <c r="AF27" s="93"/>
+      <c r="AG27" s="93"/>
+      <c r="AH27" s="93"/>
       <c r="AI27" s="94"/>
       <c r="AJ27" s="66"/>
       <c r="AK27" s="80"/>
@@ -2411,19 +2432,19 @@
       <c r="V28" s="80"/>
       <c r="W28" s="80"/>
       <c r="X28" s="67"/>
-      <c r="Y28" s="78" t="str">
-        <f>CONCATENATE("(", B28, " &lt;&lt; ", TEXT(S28, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q28) * (POWER(2, U28) - 1), 2, 24))</f>
-        <v>(c &lt;&lt; 15) &amp; 0b000001000000000000000000</v>
-      </c>
-      <c r="Z28" s="79"/>
-      <c r="AA28" s="79"/>
-      <c r="AB28" s="79"/>
-      <c r="AC28" s="79"/>
-      <c r="AD28" s="79"/>
-      <c r="AE28" s="79"/>
-      <c r="AF28" s="79"/>
-      <c r="AG28" s="79"/>
-      <c r="AH28" s="79"/>
+      <c r="Y28" s="92" t="str">
+        <f t="shared" ref="Y26:Y40" si="0">CONCATENATE("(", B28, " &lt;&lt; ", TEXT(S28, "00"), ") &amp; ", POWER(2, Q28) * (POWER(2, U28) - 1),)</f>
+        <v>(c &lt;&lt; 15) &amp; 262144</v>
+      </c>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="93"/>
+      <c r="AB28" s="93"/>
+      <c r="AC28" s="93"/>
+      <c r="AD28" s="93"/>
+      <c r="AE28" s="93"/>
+      <c r="AF28" s="93"/>
+      <c r="AG28" s="93"/>
+      <c r="AH28" s="93"/>
       <c r="AI28" s="94"/>
       <c r="AJ28" s="66" t="s">
         <v>49</v>
@@ -2452,16 +2473,16 @@
       <c r="V29" s="80"/>
       <c r="W29" s="80"/>
       <c r="X29" s="67"/>
-      <c r="Y29" s="78"/>
-      <c r="Z29" s="79"/>
-      <c r="AA29" s="79"/>
-      <c r="AB29" s="79"/>
-      <c r="AC29" s="79"/>
-      <c r="AD29" s="79"/>
-      <c r="AE29" s="79"/>
-      <c r="AF29" s="79"/>
-      <c r="AG29" s="79"/>
-      <c r="AH29" s="79"/>
+      <c r="Y29" s="92"/>
+      <c r="Z29" s="93"/>
+      <c r="AA29" s="93"/>
+      <c r="AB29" s="93"/>
+      <c r="AC29" s="93"/>
+      <c r="AD29" s="93"/>
+      <c r="AE29" s="93"/>
+      <c r="AF29" s="93"/>
+      <c r="AG29" s="93"/>
+      <c r="AH29" s="93"/>
       <c r="AI29" s="94"/>
       <c r="AJ29" s="66"/>
       <c r="AK29" s="80"/>
@@ -2514,19 +2535,19 @@
       <c r="V30" s="80"/>
       <c r="W30" s="80"/>
       <c r="X30" s="67"/>
-      <c r="Y30" s="78" t="str">
-        <f>CONCATENATE("(", B30, " &lt;&lt; ", TEXT(S30, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q30) * (POWER(2, U30) - 1), 2, 24))</f>
-        <v>(d &lt;&lt; 13) &amp; 0b000000100000000000000000</v>
-      </c>
-      <c r="Z30" s="79"/>
-      <c r="AA30" s="79"/>
-      <c r="AB30" s="79"/>
-      <c r="AC30" s="79"/>
-      <c r="AD30" s="79"/>
-      <c r="AE30" s="79"/>
-      <c r="AF30" s="79"/>
-      <c r="AG30" s="79"/>
-      <c r="AH30" s="79"/>
+      <c r="Y30" s="92" t="str">
+        <f t="shared" si="0"/>
+        <v>(d &lt;&lt; 13) &amp; 131072</v>
+      </c>
+      <c r="Z30" s="93"/>
+      <c r="AA30" s="93"/>
+      <c r="AB30" s="93"/>
+      <c r="AC30" s="93"/>
+      <c r="AD30" s="93"/>
+      <c r="AE30" s="93"/>
+      <c r="AF30" s="93"/>
+      <c r="AG30" s="93"/>
+      <c r="AH30" s="93"/>
       <c r="AI30" s="94"/>
       <c r="AJ30" s="66" t="s">
         <v>50</v>
@@ -2566,19 +2587,19 @@
       <c r="V31" s="80"/>
       <c r="W31" s="80"/>
       <c r="X31" s="67"/>
-      <c r="Y31" s="78" t="str">
-        <f>CONCATENATE("(", B30, " &lt;&lt; ", TEXT(S31, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q31) * (POWER(2, U31) - 1), 2, 24))</f>
-        <v>(d &lt;&lt; 11) &amp; 0b000000000000100000000000</v>
-      </c>
-      <c r="Z31" s="79"/>
-      <c r="AA31" s="79"/>
-      <c r="AB31" s="79"/>
-      <c r="AC31" s="79"/>
-      <c r="AD31" s="79"/>
-      <c r="AE31" s="79"/>
-      <c r="AF31" s="79"/>
-      <c r="AG31" s="79"/>
-      <c r="AH31" s="79"/>
+      <c r="Y31" s="92" t="str">
+        <f>CONCATENATE("(", B30, " &lt;&lt; ", TEXT(S31, "00"), ") &amp; ", POWER(2, Q31) * (POWER(2, U31) - 1),)</f>
+        <v>(d &lt;&lt; 11) &amp; 2048</v>
+      </c>
+      <c r="Z31" s="93"/>
+      <c r="AA31" s="93"/>
+      <c r="AB31" s="93"/>
+      <c r="AC31" s="93"/>
+      <c r="AD31" s="93"/>
+      <c r="AE31" s="93"/>
+      <c r="AF31" s="93"/>
+      <c r="AG31" s="93"/>
+      <c r="AH31" s="93"/>
       <c r="AI31" s="94"/>
       <c r="AJ31" s="66" t="s">
         <v>51</v>
@@ -2633,19 +2654,19 @@
       <c r="V32" s="80"/>
       <c r="W32" s="80"/>
       <c r="X32" s="67"/>
-      <c r="Y32" s="78" t="str">
-        <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S32, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q32) * (POWER(2, U32) - 1), 2, 24))</f>
-        <v>(e &lt;&lt; 05) &amp; 0b000000000001000000000000</v>
-      </c>
-      <c r="Z32" s="79"/>
-      <c r="AA32" s="79"/>
-      <c r="AB32" s="79"/>
-      <c r="AC32" s="79"/>
-      <c r="AD32" s="79"/>
-      <c r="AE32" s="79"/>
-      <c r="AF32" s="79"/>
-      <c r="AG32" s="79"/>
-      <c r="AH32" s="79"/>
+      <c r="Y32" s="92" t="str">
+        <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S32, "00"), ") &amp; ", POWER(2, Q32) * (POWER(2, U32) - 1),)</f>
+        <v>(e &lt;&lt; 05) &amp; 4096</v>
+      </c>
+      <c r="Z32" s="93"/>
+      <c r="AA32" s="93"/>
+      <c r="AB32" s="93"/>
+      <c r="AC32" s="93"/>
+      <c r="AD32" s="93"/>
+      <c r="AE32" s="93"/>
+      <c r="AF32" s="93"/>
+      <c r="AG32" s="93"/>
+      <c r="AH32" s="93"/>
       <c r="AI32" s="94"/>
       <c r="AJ32" s="66" t="s">
         <v>52</v>
@@ -2685,19 +2706,19 @@
       <c r="V33" s="80"/>
       <c r="W33" s="80"/>
       <c r="X33" s="67"/>
-      <c r="Y33" s="78" t="str">
-        <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S33, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q33) * (POWER(2, U33) - 1), 2, 24))</f>
-        <v>(e &lt;&lt; 03) &amp; 0b000000000000000001000000</v>
-      </c>
-      <c r="Z33" s="79"/>
-      <c r="AA33" s="79"/>
-      <c r="AB33" s="79"/>
-      <c r="AC33" s="79"/>
-      <c r="AD33" s="79"/>
-      <c r="AE33" s="79"/>
-      <c r="AF33" s="79"/>
-      <c r="AG33" s="79"/>
-      <c r="AH33" s="79"/>
+      <c r="Y33" s="92" t="str">
+        <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S33, "00"), ") &amp; ", POWER(2, Q33) * (POWER(2, U33) - 1),)</f>
+        <v>(e &lt;&lt; 03) &amp; 64</v>
+      </c>
+      <c r="Z33" s="93"/>
+      <c r="AA33" s="93"/>
+      <c r="AB33" s="93"/>
+      <c r="AC33" s="93"/>
+      <c r="AD33" s="93"/>
+      <c r="AE33" s="93"/>
+      <c r="AF33" s="93"/>
+      <c r="AG33" s="93"/>
+      <c r="AH33" s="93"/>
       <c r="AI33" s="94"/>
       <c r="AJ33" s="66" t="s">
         <v>53</v>
@@ -2750,19 +2771,19 @@
       <c r="V34" s="80"/>
       <c r="W34" s="80"/>
       <c r="X34" s="67"/>
-      <c r="Y34" s="78" t="str">
-        <f>CONCATENATE("(", B34, " &lt;&lt; ", TEXT(S34, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q34) * (POWER(2, U34) - 1), 2, 24))</f>
-        <v>(f &lt;&lt; 01) &amp; 0b000000000000000000100000</v>
-      </c>
-      <c r="Z34" s="79"/>
-      <c r="AA34" s="79"/>
-      <c r="AB34" s="79"/>
-      <c r="AC34" s="79"/>
-      <c r="AD34" s="79"/>
-      <c r="AE34" s="79"/>
-      <c r="AF34" s="79"/>
-      <c r="AG34" s="79"/>
-      <c r="AH34" s="79"/>
+      <c r="Y34" s="92" t="str">
+        <f>CONCATENATE("(", B34, " &lt;&lt; ", TEXT(S34, "00"), ") &amp; ", POWER(2, Q34) * (POWER(2, U34) - 1),)</f>
+        <v>(f &lt;&lt; 01) &amp; 32</v>
+      </c>
+      <c r="Z34" s="93"/>
+      <c r="AA34" s="93"/>
+      <c r="AB34" s="93"/>
+      <c r="AC34" s="93"/>
+      <c r="AD34" s="93"/>
+      <c r="AE34" s="93"/>
+      <c r="AF34" s="93"/>
+      <c r="AG34" s="93"/>
+      <c r="AH34" s="93"/>
       <c r="AI34" s="94"/>
       <c r="AJ34" s="66" t="s">
         <v>54</v>
@@ -2791,16 +2812,16 @@
       <c r="V35" s="80"/>
       <c r="W35" s="80"/>
       <c r="X35" s="67"/>
-      <c r="Y35" s="78"/>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="79"/>
-      <c r="AB35" s="79"/>
-      <c r="AC35" s="79"/>
-      <c r="AD35" s="79"/>
-      <c r="AE35" s="79"/>
-      <c r="AF35" s="79"/>
-      <c r="AG35" s="79"/>
-      <c r="AH35" s="79"/>
+      <c r="Y35" s="92"/>
+      <c r="Z35" s="93"/>
+      <c r="AA35" s="93"/>
+      <c r="AB35" s="93"/>
+      <c r="AC35" s="93"/>
+      <c r="AD35" s="93"/>
+      <c r="AE35" s="93"/>
+      <c r="AF35" s="93"/>
+      <c r="AG35" s="93"/>
+      <c r="AH35" s="93"/>
       <c r="AI35" s="94"/>
       <c r="AJ35" s="66"/>
       <c r="AK35" s="80"/>
@@ -2857,19 +2878,19 @@
       <c r="V36" s="80"/>
       <c r="W36" s="80"/>
       <c r="X36" s="67"/>
-      <c r="Y36" s="78" t="str">
-        <f>CONCATENATE("(", B36, " &lt;&lt; ", TEXT(S36, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q36) * (POWER(2, U36) - 1), 2, 24))</f>
-        <v>(g &lt;&lt; -03) &amp; 0b000000000000000000011110</v>
-      </c>
-      <c r="Z36" s="79"/>
-      <c r="AA36" s="79"/>
-      <c r="AB36" s="79"/>
-      <c r="AC36" s="79"/>
-      <c r="AD36" s="79"/>
-      <c r="AE36" s="79"/>
-      <c r="AF36" s="79"/>
-      <c r="AG36" s="79"/>
-      <c r="AH36" s="79"/>
+      <c r="Y36" s="92" t="str">
+        <f t="shared" si="0"/>
+        <v>(g &lt;&lt; -03) &amp; 30</v>
+      </c>
+      <c r="Z36" s="93"/>
+      <c r="AA36" s="93"/>
+      <c r="AB36" s="93"/>
+      <c r="AC36" s="93"/>
+      <c r="AD36" s="93"/>
+      <c r="AE36" s="93"/>
+      <c r="AF36" s="93"/>
+      <c r="AG36" s="93"/>
+      <c r="AH36" s="93"/>
       <c r="AI36" s="94"/>
       <c r="AJ36" s="66" t="s">
         <v>55</v>
@@ -2898,16 +2919,16 @@
       <c r="V37" s="80"/>
       <c r="W37" s="80"/>
       <c r="X37" s="67"/>
-      <c r="Y37" s="78"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-      <c r="AB37" s="79"/>
-      <c r="AC37" s="79"/>
-      <c r="AD37" s="79"/>
-      <c r="AE37" s="79"/>
-      <c r="AF37" s="79"/>
-      <c r="AG37" s="79"/>
-      <c r="AH37" s="79"/>
+      <c r="Y37" s="92"/>
+      <c r="Z37" s="93"/>
+      <c r="AA37" s="93"/>
+      <c r="AB37" s="93"/>
+      <c r="AC37" s="93"/>
+      <c r="AD37" s="93"/>
+      <c r="AE37" s="93"/>
+      <c r="AF37" s="93"/>
+      <c r="AG37" s="93"/>
+      <c r="AH37" s="93"/>
       <c r="AI37" s="94"/>
       <c r="AJ37" s="66"/>
       <c r="AK37" s="80"/>
@@ -2958,19 +2979,19 @@
       <c r="V38" s="80"/>
       <c r="W38" s="80"/>
       <c r="X38" s="67"/>
-      <c r="Y38" s="78" t="str">
-        <f>CONCATENATE("(", B38, " &lt;&lt; ", TEXT(S38, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q38) * (POWER(2, U38) - 1), 2, 24))</f>
-        <v>(h &lt;&lt; -07) &amp; 0b000000000000000000000001</v>
-      </c>
-      <c r="Z38" s="79"/>
-      <c r="AA38" s="79"/>
-      <c r="AB38" s="79"/>
-      <c r="AC38" s="79"/>
-      <c r="AD38" s="79"/>
-      <c r="AE38" s="79"/>
-      <c r="AF38" s="79"/>
-      <c r="AG38" s="79"/>
-      <c r="AH38" s="79"/>
+      <c r="Y38" s="92" t="str">
+        <f t="shared" si="0"/>
+        <v>(h &lt;&lt; -07) &amp; 1</v>
+      </c>
+      <c r="Z38" s="93"/>
+      <c r="AA38" s="93"/>
+      <c r="AB38" s="93"/>
+      <c r="AC38" s="93"/>
+      <c r="AD38" s="93"/>
+      <c r="AE38" s="93"/>
+      <c r="AF38" s="93"/>
+      <c r="AG38" s="93"/>
+      <c r="AH38" s="93"/>
       <c r="AI38" s="94"/>
       <c r="AJ38" s="66" t="s">
         <v>56</v>
@@ -2999,16 +3020,16 @@
       <c r="V39" s="80"/>
       <c r="W39" s="80"/>
       <c r="X39" s="67"/>
-      <c r="Y39" s="78"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-      <c r="AB39" s="79"/>
-      <c r="AC39" s="79"/>
-      <c r="AD39" s="79"/>
-      <c r="AE39" s="79"/>
-      <c r="AF39" s="79"/>
-      <c r="AG39" s="79"/>
-      <c r="AH39" s="79"/>
+      <c r="Y39" s="92"/>
+      <c r="Z39" s="93"/>
+      <c r="AA39" s="93"/>
+      <c r="AB39" s="93"/>
+      <c r="AC39" s="93"/>
+      <c r="AD39" s="93"/>
+      <c r="AE39" s="93"/>
+      <c r="AF39" s="93"/>
+      <c r="AG39" s="93"/>
+      <c r="AH39" s="93"/>
       <c r="AI39" s="94"/>
       <c r="AJ39" s="66"/>
       <c r="AK39" s="80"/>
@@ -3073,19 +3094,19 @@
       <c r="V40" s="80"/>
       <c r="W40" s="80"/>
       <c r="X40" s="67"/>
-      <c r="Y40" s="78" t="str">
-        <f>CONCATENATE("(", B40, " &lt;&lt; ", TEXT(S40, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q40) * (POWER(2, U40) - 1), 2, 24))</f>
-        <v>(x &lt;&lt; 09) &amp; 0b000000011110000000000000</v>
-      </c>
-      <c r="Z40" s="79"/>
-      <c r="AA40" s="79"/>
-      <c r="AB40" s="79"/>
-      <c r="AC40" s="79"/>
-      <c r="AD40" s="79"/>
-      <c r="AE40" s="79"/>
-      <c r="AF40" s="79"/>
-      <c r="AG40" s="79"/>
-      <c r="AH40" s="79"/>
+      <c r="Y40" s="92" t="str">
+        <f t="shared" si="0"/>
+        <v>(x &lt;&lt; 09) &amp; 122880</v>
+      </c>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="93"/>
+      <c r="AB40" s="93"/>
+      <c r="AC40" s="93"/>
+      <c r="AD40" s="93"/>
+      <c r="AE40" s="93"/>
+      <c r="AF40" s="93"/>
+      <c r="AG40" s="93"/>
+      <c r="AH40" s="93"/>
       <c r="AI40" s="94"/>
       <c r="AJ40" s="66" t="s">
         <v>57</v>
@@ -3122,12 +3143,12 @@
       <c r="U41" s="70">
         <v>4</v>
       </c>
-      <c r="V41" s="93"/>
-      <c r="W41" s="93"/>
+      <c r="V41" s="85"/>
+      <c r="W41" s="85"/>
       <c r="X41" s="71"/>
       <c r="Y41" s="95" t="str">
-        <f>CONCATENATE("(", B40, " &lt;&lt; ", TEXT(S41, "00"), ") &amp; 0b", _xlfn.BASE(POWER(2, Q41) * (POWER(2, U41) - 1), 2, 24))</f>
-        <v>(x &lt;&lt; 07) &amp; 0b000000000000011110000000</v>
+        <f>CONCATENATE("(", B40, " &lt;&lt; ", TEXT(S41, "00"), ") &amp; ", POWER(2, Q41) * (POWER(2, U41) - 1),)</f>
+        <v>(x &lt;&lt; 07) &amp; 1920</v>
       </c>
       <c r="Z41" s="96"/>
       <c r="AA41" s="96"/>
@@ -3142,24 +3163,19 @@
       <c r="AJ41" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="AK41" s="93"/>
-      <c r="AL41" s="93"/>
-      <c r="AM41" s="93"/>
-      <c r="AN41" s="93"/>
-      <c r="AO41" s="93"/>
-      <c r="AP41" s="93"/>
-      <c r="AQ41" s="93"/>
-      <c r="AR41" s="93"/>
-      <c r="AS41" s="93"/>
+      <c r="AK41" s="85"/>
+      <c r="AL41" s="85"/>
+      <c r="AM41" s="85"/>
+      <c r="AN41" s="85"/>
+      <c r="AO41" s="85"/>
+      <c r="AP41" s="85"/>
+      <c r="AQ41" s="85"/>
+      <c r="AR41" s="85"/>
+      <c r="AS41" s="85"/>
       <c r="AT41" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="150">
-    <mergeCell ref="AJ23:AT23"/>
-    <mergeCell ref="AJ24:AT24"/>
-    <mergeCell ref="AJ25:AT25"/>
-    <mergeCell ref="AJ26:AT26"/>
-    <mergeCell ref="AJ27:AT27"/>
     <mergeCell ref="AJ41:AT41"/>
     <mergeCell ref="AJ40:AT40"/>
     <mergeCell ref="AJ33:AT33"/>
@@ -3174,7 +3190,6 @@
     <mergeCell ref="AJ34:AT34"/>
     <mergeCell ref="AJ35:AT35"/>
     <mergeCell ref="AJ39:AT39"/>
-    <mergeCell ref="Y24:AI24"/>
     <mergeCell ref="Y25:AI25"/>
     <mergeCell ref="Y26:AI26"/>
     <mergeCell ref="Y27:AI27"/>
@@ -3183,6 +3198,11 @@
     <mergeCell ref="Y30:AI30"/>
     <mergeCell ref="Y31:AI31"/>
     <mergeCell ref="Y32:AI32"/>
+    <mergeCell ref="AJ23:AT23"/>
+    <mergeCell ref="AJ24:AT24"/>
+    <mergeCell ref="AJ25:AT25"/>
+    <mergeCell ref="AJ26:AT26"/>
+    <mergeCell ref="AJ27:AT27"/>
     <mergeCell ref="Y33:AI33"/>
     <mergeCell ref="Y34:AI34"/>
     <mergeCell ref="Y35:AI35"/>
@@ -3215,7 +3235,7 @@
     <mergeCell ref="AM5:AM6"/>
     <mergeCell ref="AN5:AN6"/>
     <mergeCell ref="Y23:AI23"/>
-    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="Y24:AI24"/>
     <mergeCell ref="S39:T39"/>
     <mergeCell ref="S40:T40"/>
     <mergeCell ref="S41:T41"/>
@@ -3237,11 +3257,6 @@
     <mergeCell ref="U39:X39"/>
     <mergeCell ref="U40:X40"/>
     <mergeCell ref="U41:X41"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O32:P32"/>
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
@@ -3250,8 +3265,19 @@
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="U32:X32"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U34:X34"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U36:X36"/>
+    <mergeCell ref="U38:X38"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="O32:P32"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O26:P26"/>
@@ -3263,14 +3289,7 @@
     <mergeCell ref="U29:X29"/>
     <mergeCell ref="U30:X30"/>
     <mergeCell ref="U31:X31"/>
-    <mergeCell ref="U32:X32"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U34:X34"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="U38:X38"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="O29:P29"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="M35:N35"/>
     <mergeCell ref="M32:N32"/>
@@ -3281,6 +3300,8 @@
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O35:P35"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="M41:N41"/>
     <mergeCell ref="O41:P41"/>

</xml_diff>

<commit_message>
It works I guess...
</commit_message>
<xml_diff>
--- a/Assets/Docs/LookupTables.xlsx
+++ b/Assets/Docs/LookupTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Lookup table:</t>
   </si>
@@ -161,9 +161,6 @@
     <t>significant bits</t>
   </si>
   <si>
-    <t>(b &lt;&lt; 19) &amp; 0b11110000000000000000000</t>
-  </si>
-  <si>
     <t>final</t>
   </si>
   <si>
@@ -203,10 +200,43 @@
     <t>(x &lt;&lt; 07) &amp; 1920</t>
   </si>
   <si>
-    <t>Get local bit:</t>
-  </si>
-  <si>
-    <t>(chunkData &gt;&gt; (7 - x - 4 * y)) &amp; 1</t>
+    <t>Packed Lookup Table element (int):</t>
+  </si>
+  <si>
+    <t>Packing:</t>
+  </si>
+  <si>
+    <t>Unpacking:</t>
+  </si>
+  <si>
+    <t>(byte0 &lt;&lt; 0) +</t>
+  </si>
+  <si>
+    <t>(byte1 &lt;&lt; 8) +</t>
+  </si>
+  <si>
+    <t>(byte2 &lt;&lt; 16) +</t>
+  </si>
+  <si>
+    <t>(byte3 &lt;&lt; 24)</t>
+  </si>
+  <si>
+    <t>Unpack byteN:</t>
+  </si>
+  <si>
+    <t>byte0 = (data &gt;&gt; 0) &amp; 255</t>
+  </si>
+  <si>
+    <t>byte1 = (data &gt;&gt; 8) &amp; 255</t>
+  </si>
+  <si>
+    <t>byte2 = (data &gt;&gt; 16) &amp; 255</t>
+  </si>
+  <si>
+    <t>byte3 = (data &gt;&gt; 24) &amp; 255</t>
+  </si>
+  <si>
+    <t>byteN = (data &gt;&gt; (n * 8)) &amp; 255</t>
   </si>
 </sst>
 </file>
@@ -254,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +315,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -662,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -859,6 +913,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -937,6 +1006,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -953,15 +1031,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -995,7 +1064,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>7798</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>12112</xdr:rowOff>
+      <xdr:rowOff>5952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
@@ -1010,8 +1079,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="757892" y="10513425"/>
-          <a:ext cx="4248000" cy="3500437"/>
+          <a:off x="757892" y="10507265"/>
+          <a:ext cx="4248000" cy="3506597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1521,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AT41"/>
+  <dimension ref="B1:AT67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27:AI27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1581,28 +1650,28 @@
       <c r="O5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AI5" s="86" t="s">
+      <c r="AI5" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="AJ5" s="86" t="s">
+      <c r="AJ5" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="AK5" s="86" t="s">
+      <c r="AK5" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="AL5" s="86" t="s">
+      <c r="AL5" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="86" t="s">
+      <c r="AM5" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="AN5" s="86" t="s">
+      <c r="AN5" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="AO5" s="86" t="s">
+      <c r="AO5" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="AP5" s="86" t="s">
+      <c r="AP5" s="91" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1645,14 +1714,14 @@
       </c>
       <c r="AF6" s="52"/>
       <c r="AG6" s="44"/>
-      <c r="AI6" s="87"/>
-      <c r="AJ6" s="87"/>
-      <c r="AK6" s="87"/>
-      <c r="AL6" s="87"/>
-      <c r="AM6" s="87"/>
-      <c r="AN6" s="87"/>
-      <c r="AO6" s="87"/>
-      <c r="AP6" s="87"/>
+      <c r="AI6" s="92"/>
+      <c r="AJ6" s="92"/>
+      <c r="AK6" s="92"/>
+      <c r="AL6" s="92"/>
+      <c r="AM6" s="92"/>
+      <c r="AN6" s="92"/>
+      <c r="AO6" s="92"/>
+      <c r="AP6" s="92"/>
     </row>
     <row r="7" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
@@ -1678,10 +1747,10 @@
       </c>
       <c r="N7" s="44"/>
       <c r="O7" s="44"/>
-      <c r="R7" s="90" t="s">
+      <c r="R7" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="90"/>
+      <c r="S7" s="95"/>
       <c r="AB7" s="49">
         <v>0</v>
       </c>
@@ -1748,8 +1817,8 @@
       <c r="J8" s="7"/>
       <c r="N8" s="45"/>
       <c r="O8" s="45"/>
-      <c r="R8" s="91"/>
-      <c r="S8" s="91"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="96"/>
     </row>
     <row r="9" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
@@ -1772,29 +1841,27 @@
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="16"/>
-      <c r="N9" s="72" t="s">
+      <c r="N9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="73"/>
+      <c r="O9" s="78"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="18"/>
       <c r="U9" s="16"/>
-      <c r="V9" s="72" t="s">
+      <c r="V9" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="W9" s="73"/>
+      <c r="W9" s="78"/>
       <c r="X9" s="18"/>
-      <c r="AB9" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB9" s="8"/>
     </row>
     <row r="10" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M10" s="19"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="75"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="21">
         <v>18</v>
       </c>
@@ -1813,22 +1880,20 @@
       <c r="U10" s="29">
         <v>23</v>
       </c>
-      <c r="V10" s="74"/>
-      <c r="W10" s="75"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="80"/>
       <c r="X10" s="22"/>
-      <c r="AB10" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="AB10" s="8"/>
     </row>
     <row r="11" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="M11" s="16"/>
-      <c r="N11" s="72" t="s">
+      <c r="N11" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="73"/>
+      <c r="O11" s="78"/>
       <c r="P11" s="34">
         <v>12</v>
       </c>
@@ -1847,17 +1912,17 @@
       <c r="U11" s="35">
         <v>17</v>
       </c>
-      <c r="V11" s="72" t="s">
+      <c r="V11" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="W11" s="73"/>
+      <c r="W11" s="78"/>
       <c r="X11" s="18"/>
     </row>
     <row r="12" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12" s="8"/>
       <c r="M12" s="19"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="75"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="80"/>
       <c r="P12" s="21">
         <v>6</v>
       </c>
@@ -1876,8 +1941,8 @@
       <c r="U12" s="29">
         <v>11</v>
       </c>
-      <c r="V12" s="74"/>
-      <c r="W12" s="75"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="80"/>
       <c r="X12" s="22"/>
     </row>
     <row r="13" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1886,10 +1951,10 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="72" t="s">
+      <c r="N13" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="73"/>
+      <c r="O13" s="78"/>
       <c r="P13" s="34">
         <v>0</v>
       </c>
@@ -1908,10 +1973,10 @@
       <c r="U13" s="35">
         <v>5</v>
       </c>
-      <c r="V13" s="72" t="s">
+      <c r="V13" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="W13" s="73"/>
+      <c r="W13" s="78"/>
       <c r="X13" s="18"/>
     </row>
     <row r="14" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,28 +1985,28 @@
       <c r="E14" s="15"/>
       <c r="F14" s="14"/>
       <c r="M14" s="19"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="75"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="80"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
       <c r="T14" s="22"/>
       <c r="U14" s="19"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="75"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="80"/>
       <c r="X14" s="22"/>
     </row>
     <row r="15" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R15" s="88" t="s">
+      <c r="R15" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="S15" s="88"/>
+      <c r="S15" s="93"/>
       <c r="AA15" s="8"/>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R16" s="89"/>
-      <c r="S16" s="89"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="94"/>
       <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2098,20 +2163,18 @@
     <row r="20" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T20" s="8"/>
       <c r="Y20" s="8"/>
-      <c r="AA20" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA20" s="8"/>
     </row>
     <row r="21" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22" s="78" t="s">
+      <c r="O22" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="79"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="86"/>
+      <c r="R22" s="84"/>
     </row>
     <row r="23" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D23" s="65">
@@ -2138,54 +2201,54 @@
       <c r="K23" s="65">
         <v>0</v>
       </c>
-      <c r="M23" s="78" t="s">
+      <c r="M23" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="N23" s="79"/>
-      <c r="O23" s="78" t="s">
+      <c r="N23" s="84"/>
+      <c r="O23" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="78" t="s">
+      <c r="P23" s="84"/>
+      <c r="Q23" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="79"/>
-      <c r="S23" s="78" t="s">
+      <c r="R23" s="84"/>
+      <c r="S23" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="T23" s="79"/>
-      <c r="U23" s="78" t="s">
+      <c r="T23" s="84"/>
+      <c r="U23" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="78" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z23" s="81"/>
-      <c r="AA23" s="81"/>
-      <c r="AB23" s="81"/>
-      <c r="AC23" s="81"/>
-      <c r="AD23" s="81"/>
-      <c r="AE23" s="81"/>
-      <c r="AF23" s="81"/>
-      <c r="AG23" s="81"/>
-      <c r="AH23" s="81"/>
-      <c r="AI23" s="79"/>
-      <c r="AJ23" s="78" t="s">
+      <c r="V23" s="86"/>
+      <c r="W23" s="86"/>
+      <c r="X23" s="84"/>
+      <c r="Y23" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z23" s="86"/>
+      <c r="AA23" s="86"/>
+      <c r="AB23" s="86"/>
+      <c r="AC23" s="86"/>
+      <c r="AD23" s="86"/>
+      <c r="AE23" s="86"/>
+      <c r="AF23" s="86"/>
+      <c r="AG23" s="86"/>
+      <c r="AH23" s="86"/>
+      <c r="AI23" s="84"/>
+      <c r="AJ23" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="AK23" s="81"/>
-      <c r="AL23" s="81"/>
-      <c r="AM23" s="81"/>
-      <c r="AN23" s="81"/>
-      <c r="AO23" s="81"/>
-      <c r="AP23" s="81"/>
-      <c r="AQ23" s="81"/>
-      <c r="AR23" s="81"/>
-      <c r="AS23" s="81"/>
-      <c r="AT23" s="79"/>
+      <c r="AK23" s="86"/>
+      <c r="AL23" s="86"/>
+      <c r="AM23" s="86"/>
+      <c r="AN23" s="86"/>
+      <c r="AO23" s="86"/>
+      <c r="AP23" s="86"/>
+      <c r="AQ23" s="86"/>
+      <c r="AR23" s="86"/>
+      <c r="AS23" s="86"/>
+      <c r="AT23" s="84"/>
     </row>
     <row r="24" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -2201,92 +2264,92 @@
       <c r="K24" s="26">
         <v>0</v>
       </c>
-      <c r="M24" s="76" t="s">
+      <c r="M24" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="N24" s="77"/>
-      <c r="O24" s="66">
+      <c r="N24" s="82"/>
+      <c r="O24" s="71">
         <v>0</v>
       </c>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="66">
+      <c r="P24" s="72"/>
+      <c r="Q24" s="71">
         <v>23</v>
       </c>
-      <c r="R24" s="67"/>
-      <c r="S24" s="66">
+      <c r="R24" s="72"/>
+      <c r="S24" s="71">
         <f>Q24-O24</f>
         <v>23</v>
       </c>
-      <c r="T24" s="67"/>
-      <c r="U24" s="82">
+      <c r="T24" s="72"/>
+      <c r="U24" s="87">
         <v>1</v>
       </c>
-      <c r="V24" s="83"/>
-      <c r="W24" s="83"/>
-      <c r="X24" s="84"/>
-      <c r="Y24" s="98" t="str">
+      <c r="V24" s="88"/>
+      <c r="W24" s="88"/>
+      <c r="X24" s="89"/>
+      <c r="Y24" s="97" t="str">
         <f>CONCATENATE("(", B24, " &lt;&lt; ", TEXT(S24, "00"), ") &amp; ", POWER(2, Q24) * (POWER(2, U24) - 1),)</f>
         <v>(a &lt;&lt; 23) &amp; 8388608</v>
       </c>
-      <c r="Z24" s="99"/>
-      <c r="AA24" s="99"/>
-      <c r="AB24" s="99"/>
-      <c r="AC24" s="99"/>
-      <c r="AD24" s="99"/>
-      <c r="AE24" s="99"/>
-      <c r="AF24" s="99"/>
-      <c r="AG24" s="99"/>
-      <c r="AH24" s="99"/>
-      <c r="AI24" s="100"/>
-      <c r="AJ24" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK24" s="83"/>
-      <c r="AL24" s="83"/>
-      <c r="AM24" s="83"/>
-      <c r="AN24" s="83"/>
-      <c r="AO24" s="83"/>
-      <c r="AP24" s="83"/>
-      <c r="AQ24" s="83"/>
-      <c r="AR24" s="83"/>
-      <c r="AS24" s="83"/>
-      <c r="AT24" s="84"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="98"/>
+      <c r="AB24" s="98"/>
+      <c r="AC24" s="98"/>
+      <c r="AD24" s="98"/>
+      <c r="AE24" s="98"/>
+      <c r="AF24" s="98"/>
+      <c r="AG24" s="98"/>
+      <c r="AH24" s="98"/>
+      <c r="AI24" s="99"/>
+      <c r="AJ24" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK24" s="88"/>
+      <c r="AL24" s="88"/>
+      <c r="AM24" s="88"/>
+      <c r="AN24" s="88"/>
+      <c r="AO24" s="88"/>
+      <c r="AP24" s="88"/>
+      <c r="AQ24" s="88"/>
+      <c r="AR24" s="88"/>
+      <c r="AS24" s="88"/>
+      <c r="AT24" s="89"/>
     </row>
     <row r="25" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M25" s="76"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="66"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="66"/>
-      <c r="T25" s="67"/>
-      <c r="U25" s="66"/>
-      <c r="V25" s="80"/>
-      <c r="W25" s="80"/>
-      <c r="X25" s="67"/>
-      <c r="Y25" s="92"/>
-      <c r="Z25" s="93"/>
-      <c r="AA25" s="93"/>
-      <c r="AB25" s="93"/>
-      <c r="AC25" s="93"/>
-      <c r="AD25" s="93"/>
-      <c r="AE25" s="93"/>
-      <c r="AF25" s="93"/>
-      <c r="AG25" s="93"/>
-      <c r="AH25" s="93"/>
-      <c r="AI25" s="94"/>
-      <c r="AJ25" s="66"/>
-      <c r="AK25" s="80"/>
-      <c r="AL25" s="80"/>
-      <c r="AM25" s="80"/>
-      <c r="AN25" s="80"/>
-      <c r="AO25" s="80"/>
-      <c r="AP25" s="80"/>
-      <c r="AQ25" s="80"/>
-      <c r="AR25" s="80"/>
-      <c r="AS25" s="80"/>
-      <c r="AT25" s="67"/>
+      <c r="M25" s="81"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="72"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="72"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="72"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="85"/>
+      <c r="W25" s="85"/>
+      <c r="X25" s="72"/>
+      <c r="Y25" s="100"/>
+      <c r="Z25" s="101"/>
+      <c r="AA25" s="101"/>
+      <c r="AB25" s="101"/>
+      <c r="AC25" s="101"/>
+      <c r="AD25" s="101"/>
+      <c r="AE25" s="101"/>
+      <c r="AF25" s="101"/>
+      <c r="AG25" s="101"/>
+      <c r="AH25" s="101"/>
+      <c r="AI25" s="102"/>
+      <c r="AJ25" s="71"/>
+      <c r="AK25" s="85"/>
+      <c r="AL25" s="85"/>
+      <c r="AM25" s="85"/>
+      <c r="AN25" s="85"/>
+      <c r="AO25" s="85"/>
+      <c r="AP25" s="85"/>
+      <c r="AQ25" s="85"/>
+      <c r="AR25" s="85"/>
+      <c r="AS25" s="85"/>
+      <c r="AT25" s="72"/>
     </row>
     <row r="26" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
@@ -2308,92 +2371,92 @@
       <c r="K26" s="56">
         <v>4</v>
       </c>
-      <c r="M26" s="76" t="s">
+      <c r="M26" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N26" s="77"/>
-      <c r="O26" s="66">
+      <c r="N26" s="82"/>
+      <c r="O26" s="71">
         <v>0</v>
       </c>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="66">
+      <c r="P26" s="72"/>
+      <c r="Q26" s="71">
         <v>19</v>
       </c>
-      <c r="R26" s="67"/>
-      <c r="S26" s="66">
+      <c r="R26" s="72"/>
+      <c r="S26" s="71">
         <f>Q26-O26</f>
         <v>19</v>
       </c>
-      <c r="T26" s="67"/>
-      <c r="U26" s="66">
+      <c r="T26" s="72"/>
+      <c r="U26" s="71">
         <v>4</v>
       </c>
-      <c r="V26" s="80"/>
-      <c r="W26" s="80"/>
-      <c r="X26" s="67"/>
-      <c r="Y26" s="92" t="str">
+      <c r="V26" s="85"/>
+      <c r="W26" s="85"/>
+      <c r="X26" s="72"/>
+      <c r="Y26" s="100" t="str">
         <f>CONCATENATE("(", B26, " &lt;&lt; ", TEXT(S26, "00"), ") &amp; ", POWER(2, Q26) * (POWER(2, U26) - 1),)</f>
         <v>(b &lt;&lt; 19) &amp; 7864320</v>
       </c>
-      <c r="Z26" s="93"/>
-      <c r="AA26" s="93"/>
-      <c r="AB26" s="93"/>
-      <c r="AC26" s="93"/>
-      <c r="AD26" s="93"/>
-      <c r="AE26" s="93"/>
-      <c r="AF26" s="93"/>
-      <c r="AG26" s="93"/>
-      <c r="AH26" s="93"/>
-      <c r="AI26" s="94"/>
-      <c r="AJ26" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK26" s="80"/>
-      <c r="AL26" s="80"/>
-      <c r="AM26" s="80"/>
-      <c r="AN26" s="80"/>
-      <c r="AO26" s="80"/>
-      <c r="AP26" s="80"/>
-      <c r="AQ26" s="80"/>
-      <c r="AR26" s="80"/>
-      <c r="AS26" s="80"/>
-      <c r="AT26" s="67"/>
+      <c r="Z26" s="101"/>
+      <c r="AA26" s="101"/>
+      <c r="AB26" s="101"/>
+      <c r="AC26" s="101"/>
+      <c r="AD26" s="101"/>
+      <c r="AE26" s="101"/>
+      <c r="AF26" s="101"/>
+      <c r="AG26" s="101"/>
+      <c r="AH26" s="101"/>
+      <c r="AI26" s="102"/>
+      <c r="AJ26" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK26" s="85"/>
+      <c r="AL26" s="85"/>
+      <c r="AM26" s="85"/>
+      <c r="AN26" s="85"/>
+      <c r="AO26" s="85"/>
+      <c r="AP26" s="85"/>
+      <c r="AQ26" s="85"/>
+      <c r="AR26" s="85"/>
+      <c r="AS26" s="85"/>
+      <c r="AT26" s="72"/>
     </row>
     <row r="27" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M27" s="76"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="67"/>
-      <c r="Q27" s="66"/>
-      <c r="R27" s="67"/>
-      <c r="S27" s="66"/>
-      <c r="T27" s="67"/>
-      <c r="U27" s="66"/>
-      <c r="V27" s="80"/>
-      <c r="W27" s="80"/>
-      <c r="X27" s="67"/>
-      <c r="Y27" s="92"/>
-      <c r="Z27" s="93"/>
-      <c r="AA27" s="93"/>
-      <c r="AB27" s="93"/>
-      <c r="AC27" s="93"/>
-      <c r="AD27" s="93"/>
-      <c r="AE27" s="93"/>
-      <c r="AF27" s="93"/>
-      <c r="AG27" s="93"/>
-      <c r="AH27" s="93"/>
-      <c r="AI27" s="94"/>
-      <c r="AJ27" s="66"/>
-      <c r="AK27" s="80"/>
-      <c r="AL27" s="80"/>
-      <c r="AM27" s="80"/>
-      <c r="AN27" s="80"/>
-      <c r="AO27" s="80"/>
-      <c r="AP27" s="80"/>
-      <c r="AQ27" s="80"/>
-      <c r="AR27" s="80"/>
-      <c r="AS27" s="80"/>
-      <c r="AT27" s="67"/>
+      <c r="M27" s="81"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="71"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="71"/>
+      <c r="V27" s="85"/>
+      <c r="W27" s="85"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="101"/>
+      <c r="AA27" s="101"/>
+      <c r="AB27" s="101"/>
+      <c r="AC27" s="101"/>
+      <c r="AD27" s="101"/>
+      <c r="AE27" s="101"/>
+      <c r="AF27" s="101"/>
+      <c r="AG27" s="101"/>
+      <c r="AH27" s="101"/>
+      <c r="AI27" s="102"/>
+      <c r="AJ27" s="71"/>
+      <c r="AK27" s="85"/>
+      <c r="AL27" s="85"/>
+      <c r="AM27" s="85"/>
+      <c r="AN27" s="85"/>
+      <c r="AO27" s="85"/>
+      <c r="AP27" s="85"/>
+      <c r="AQ27" s="85"/>
+      <c r="AR27" s="85"/>
+      <c r="AS27" s="85"/>
+      <c r="AT27" s="72"/>
     </row>
     <row r="28" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
@@ -2409,92 +2472,92 @@
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
       <c r="K28" s="27"/>
-      <c r="M28" s="76" t="s">
+      <c r="M28" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="N28" s="77"/>
-      <c r="O28" s="66">
+      <c r="N28" s="82"/>
+      <c r="O28" s="71">
         <v>3</v>
       </c>
-      <c r="P28" s="67"/>
-      <c r="Q28" s="66">
+      <c r="P28" s="72"/>
+      <c r="Q28" s="71">
         <v>18</v>
       </c>
-      <c r="R28" s="67"/>
-      <c r="S28" s="66">
+      <c r="R28" s="72"/>
+      <c r="S28" s="71">
         <f>Q28-O28</f>
         <v>15</v>
       </c>
-      <c r="T28" s="67"/>
-      <c r="U28" s="66">
+      <c r="T28" s="72"/>
+      <c r="U28" s="71">
         <v>1</v>
       </c>
-      <c r="V28" s="80"/>
-      <c r="W28" s="80"/>
-      <c r="X28" s="67"/>
-      <c r="Y28" s="92" t="str">
-        <f t="shared" ref="Y26:Y40" si="0">CONCATENATE("(", B28, " &lt;&lt; ", TEXT(S28, "00"), ") &amp; ", POWER(2, Q28) * (POWER(2, U28) - 1),)</f>
+      <c r="V28" s="85"/>
+      <c r="W28" s="85"/>
+      <c r="X28" s="72"/>
+      <c r="Y28" s="100" t="str">
+        <f t="shared" ref="Y28:Y40" si="0">CONCATENATE("(", B28, " &lt;&lt; ", TEXT(S28, "00"), ") &amp; ", POWER(2, Q28) * (POWER(2, U28) - 1),)</f>
         <v>(c &lt;&lt; 15) &amp; 262144</v>
       </c>
-      <c r="Z28" s="93"/>
-      <c r="AA28" s="93"/>
-      <c r="AB28" s="93"/>
-      <c r="AC28" s="93"/>
-      <c r="AD28" s="93"/>
-      <c r="AE28" s="93"/>
-      <c r="AF28" s="93"/>
-      <c r="AG28" s="93"/>
-      <c r="AH28" s="93"/>
-      <c r="AI28" s="94"/>
-      <c r="AJ28" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK28" s="80"/>
-      <c r="AL28" s="80"/>
-      <c r="AM28" s="80"/>
-      <c r="AN28" s="80"/>
-      <c r="AO28" s="80"/>
-      <c r="AP28" s="80"/>
-      <c r="AQ28" s="80"/>
-      <c r="AR28" s="80"/>
-      <c r="AS28" s="80"/>
-      <c r="AT28" s="67"/>
+      <c r="Z28" s="101"/>
+      <c r="AA28" s="101"/>
+      <c r="AB28" s="101"/>
+      <c r="AC28" s="101"/>
+      <c r="AD28" s="101"/>
+      <c r="AE28" s="101"/>
+      <c r="AF28" s="101"/>
+      <c r="AG28" s="101"/>
+      <c r="AH28" s="101"/>
+      <c r="AI28" s="102"/>
+      <c r="AJ28" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK28" s="85"/>
+      <c r="AL28" s="85"/>
+      <c r="AM28" s="85"/>
+      <c r="AN28" s="85"/>
+      <c r="AO28" s="85"/>
+      <c r="AP28" s="85"/>
+      <c r="AQ28" s="85"/>
+      <c r="AR28" s="85"/>
+      <c r="AS28" s="85"/>
+      <c r="AT28" s="72"/>
     </row>
     <row r="29" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M29" s="76"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="66"/>
-      <c r="P29" s="67"/>
-      <c r="Q29" s="66"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="66"/>
-      <c r="T29" s="67"/>
-      <c r="U29" s="66"/>
-      <c r="V29" s="80"/>
-      <c r="W29" s="80"/>
-      <c r="X29" s="67"/>
-      <c r="Y29" s="92"/>
-      <c r="Z29" s="93"/>
-      <c r="AA29" s="93"/>
-      <c r="AB29" s="93"/>
-      <c r="AC29" s="93"/>
-      <c r="AD29" s="93"/>
-      <c r="AE29" s="93"/>
-      <c r="AF29" s="93"/>
-      <c r="AG29" s="93"/>
-      <c r="AH29" s="93"/>
-      <c r="AI29" s="94"/>
-      <c r="AJ29" s="66"/>
-      <c r="AK29" s="80"/>
-      <c r="AL29" s="80"/>
-      <c r="AM29" s="80"/>
-      <c r="AN29" s="80"/>
-      <c r="AO29" s="80"/>
-      <c r="AP29" s="80"/>
-      <c r="AQ29" s="80"/>
-      <c r="AR29" s="80"/>
-      <c r="AS29" s="80"/>
-      <c r="AT29" s="67"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="71"/>
+      <c r="R29" s="72"/>
+      <c r="S29" s="71"/>
+      <c r="T29" s="72"/>
+      <c r="U29" s="71"/>
+      <c r="V29" s="85"/>
+      <c r="W29" s="85"/>
+      <c r="X29" s="72"/>
+      <c r="Y29" s="100"/>
+      <c r="Z29" s="101"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="101"/>
+      <c r="AD29" s="101"/>
+      <c r="AE29" s="101"/>
+      <c r="AF29" s="101"/>
+      <c r="AG29" s="101"/>
+      <c r="AH29" s="101"/>
+      <c r="AI29" s="102"/>
+      <c r="AJ29" s="71"/>
+      <c r="AK29" s="85"/>
+      <c r="AL29" s="85"/>
+      <c r="AM29" s="85"/>
+      <c r="AN29" s="85"/>
+      <c r="AO29" s="85"/>
+      <c r="AP29" s="85"/>
+      <c r="AQ29" s="85"/>
+      <c r="AR29" s="85"/>
+      <c r="AS29" s="85"/>
+      <c r="AT29" s="72"/>
     </row>
     <row r="30" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -2512,108 +2575,108 @@
       <c r="K30" s="26">
         <v>12</v>
       </c>
-      <c r="M30" s="76" t="s">
+      <c r="M30" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="N30" s="77"/>
-      <c r="O30" s="66">
+      <c r="N30" s="82"/>
+      <c r="O30" s="71">
         <v>4</v>
       </c>
-      <c r="P30" s="67"/>
-      <c r="Q30" s="66">
+      <c r="P30" s="72"/>
+      <c r="Q30" s="71">
         <v>17</v>
       </c>
-      <c r="R30" s="67"/>
-      <c r="S30" s="66">
+      <c r="R30" s="72"/>
+      <c r="S30" s="71">
         <f>Q30-O30</f>
         <v>13</v>
       </c>
-      <c r="T30" s="67"/>
-      <c r="U30" s="66">
+      <c r="T30" s="72"/>
+      <c r="U30" s="71">
         <v>1</v>
       </c>
-      <c r="V30" s="80"/>
-      <c r="W30" s="80"/>
-      <c r="X30" s="67"/>
-      <c r="Y30" s="92" t="str">
+      <c r="V30" s="85"/>
+      <c r="W30" s="85"/>
+      <c r="X30" s="72"/>
+      <c r="Y30" s="100" t="str">
         <f t="shared" si="0"/>
         <v>(d &lt;&lt; 13) &amp; 131072</v>
       </c>
-      <c r="Z30" s="93"/>
-      <c r="AA30" s="93"/>
-      <c r="AB30" s="93"/>
-      <c r="AC30" s="93"/>
-      <c r="AD30" s="93"/>
-      <c r="AE30" s="93"/>
-      <c r="AF30" s="93"/>
-      <c r="AG30" s="93"/>
-      <c r="AH30" s="93"/>
-      <c r="AI30" s="94"/>
-      <c r="AJ30" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK30" s="80"/>
-      <c r="AL30" s="80"/>
-      <c r="AM30" s="80"/>
-      <c r="AN30" s="80"/>
-      <c r="AO30" s="80"/>
-      <c r="AP30" s="80"/>
-      <c r="AQ30" s="80"/>
-      <c r="AR30" s="80"/>
-      <c r="AS30" s="80"/>
-      <c r="AT30" s="67"/>
+      <c r="Z30" s="101"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="101"/>
+      <c r="AC30" s="101"/>
+      <c r="AD30" s="101"/>
+      <c r="AE30" s="101"/>
+      <c r="AF30" s="101"/>
+      <c r="AG30" s="101"/>
+      <c r="AH30" s="101"/>
+      <c r="AI30" s="102"/>
+      <c r="AJ30" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK30" s="85"/>
+      <c r="AL30" s="85"/>
+      <c r="AM30" s="85"/>
+      <c r="AN30" s="85"/>
+      <c r="AO30" s="85"/>
+      <c r="AP30" s="85"/>
+      <c r="AQ30" s="85"/>
+      <c r="AR30" s="85"/>
+      <c r="AS30" s="85"/>
+      <c r="AT30" s="72"/>
     </row>
     <row r="31" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M31" s="76" t="s">
+      <c r="M31" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="N31" s="77"/>
-      <c r="O31" s="66">
+      <c r="N31" s="82"/>
+      <c r="O31" s="71">
         <v>0</v>
       </c>
-      <c r="P31" s="67"/>
-      <c r="Q31" s="66">
+      <c r="P31" s="72"/>
+      <c r="Q31" s="71">
         <v>11</v>
       </c>
-      <c r="R31" s="67"/>
-      <c r="S31" s="66">
+      <c r="R31" s="72"/>
+      <c r="S31" s="71">
         <f>Q31-O31</f>
         <v>11</v>
       </c>
-      <c r="T31" s="67"/>
-      <c r="U31" s="66">
+      <c r="T31" s="72"/>
+      <c r="U31" s="71">
         <v>1</v>
       </c>
-      <c r="V31" s="80"/>
-      <c r="W31" s="80"/>
-      <c r="X31" s="67"/>
-      <c r="Y31" s="92" t="str">
+      <c r="V31" s="85"/>
+      <c r="W31" s="85"/>
+      <c r="X31" s="72"/>
+      <c r="Y31" s="100" t="str">
         <f>CONCATENATE("(", B30, " &lt;&lt; ", TEXT(S31, "00"), ") &amp; ", POWER(2, Q31) * (POWER(2, U31) - 1),)</f>
         <v>(d &lt;&lt; 11) &amp; 2048</v>
       </c>
-      <c r="Z31" s="93"/>
-      <c r="AA31" s="93"/>
-      <c r="AB31" s="93"/>
-      <c r="AC31" s="93"/>
-      <c r="AD31" s="93"/>
-      <c r="AE31" s="93"/>
-      <c r="AF31" s="93"/>
-      <c r="AG31" s="93"/>
-      <c r="AH31" s="93"/>
-      <c r="AI31" s="94"/>
-      <c r="AJ31" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK31" s="80"/>
-      <c r="AL31" s="80"/>
-      <c r="AM31" s="80"/>
-      <c r="AN31" s="80"/>
-      <c r="AO31" s="80"/>
-      <c r="AP31" s="80"/>
-      <c r="AQ31" s="80"/>
-      <c r="AR31" s="80"/>
-      <c r="AS31" s="80"/>
-      <c r="AT31" s="67"/>
+      <c r="Z31" s="101"/>
+      <c r="AA31" s="101"/>
+      <c r="AB31" s="101"/>
+      <c r="AC31" s="101"/>
+      <c r="AD31" s="101"/>
+      <c r="AE31" s="101"/>
+      <c r="AF31" s="101"/>
+      <c r="AG31" s="101"/>
+      <c r="AH31" s="101"/>
+      <c r="AI31" s="102"/>
+      <c r="AJ31" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK31" s="85"/>
+      <c r="AL31" s="85"/>
+      <c r="AM31" s="85"/>
+      <c r="AN31" s="85"/>
+      <c r="AO31" s="85"/>
+      <c r="AP31" s="85"/>
+      <c r="AQ31" s="85"/>
+      <c r="AR31" s="85"/>
+      <c r="AS31" s="85"/>
+      <c r="AT31" s="72"/>
     </row>
     <row r="32" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
@@ -2631,108 +2694,108 @@
       <c r="I32" s="24"/>
       <c r="J32" s="24"/>
       <c r="K32" s="27"/>
-      <c r="M32" s="76" t="s">
+      <c r="M32" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="N32" s="77"/>
-      <c r="O32" s="66">
+      <c r="N32" s="82"/>
+      <c r="O32" s="71">
         <v>7</v>
       </c>
-      <c r="P32" s="67"/>
-      <c r="Q32" s="66">
+      <c r="P32" s="72"/>
+      <c r="Q32" s="71">
         <v>12</v>
       </c>
-      <c r="R32" s="67"/>
-      <c r="S32" s="66">
+      <c r="R32" s="72"/>
+      <c r="S32" s="71">
         <f>Q32-O32</f>
         <v>5</v>
       </c>
-      <c r="T32" s="67"/>
-      <c r="U32" s="66">
+      <c r="T32" s="72"/>
+      <c r="U32" s="71">
         <v>1</v>
       </c>
-      <c r="V32" s="80"/>
-      <c r="W32" s="80"/>
-      <c r="X32" s="67"/>
-      <c r="Y32" s="92" t="str">
+      <c r="V32" s="85"/>
+      <c r="W32" s="85"/>
+      <c r="X32" s="72"/>
+      <c r="Y32" s="100" t="str">
         <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S32, "00"), ") &amp; ", POWER(2, Q32) * (POWER(2, U32) - 1),)</f>
         <v>(e &lt;&lt; 05) &amp; 4096</v>
       </c>
-      <c r="Z32" s="93"/>
-      <c r="AA32" s="93"/>
-      <c r="AB32" s="93"/>
-      <c r="AC32" s="93"/>
-      <c r="AD32" s="93"/>
-      <c r="AE32" s="93"/>
-      <c r="AF32" s="93"/>
-      <c r="AG32" s="93"/>
-      <c r="AH32" s="93"/>
-      <c r="AI32" s="94"/>
-      <c r="AJ32" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK32" s="80"/>
-      <c r="AL32" s="80"/>
-      <c r="AM32" s="80"/>
-      <c r="AN32" s="80"/>
-      <c r="AO32" s="80"/>
-      <c r="AP32" s="80"/>
-      <c r="AQ32" s="80"/>
-      <c r="AR32" s="80"/>
-      <c r="AS32" s="80"/>
-      <c r="AT32" s="67"/>
+      <c r="Z32" s="101"/>
+      <c r="AA32" s="101"/>
+      <c r="AB32" s="101"/>
+      <c r="AC32" s="101"/>
+      <c r="AD32" s="101"/>
+      <c r="AE32" s="101"/>
+      <c r="AF32" s="101"/>
+      <c r="AG32" s="101"/>
+      <c r="AH32" s="101"/>
+      <c r="AI32" s="102"/>
+      <c r="AJ32" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK32" s="85"/>
+      <c r="AL32" s="85"/>
+      <c r="AM32" s="85"/>
+      <c r="AN32" s="85"/>
+      <c r="AO32" s="85"/>
+      <c r="AP32" s="85"/>
+      <c r="AQ32" s="85"/>
+      <c r="AR32" s="85"/>
+      <c r="AS32" s="85"/>
+      <c r="AT32" s="72"/>
     </row>
     <row r="33" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M33" s="76" t="s">
+      <c r="M33" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="N33" s="77"/>
-      <c r="O33" s="66">
+      <c r="N33" s="82"/>
+      <c r="O33" s="71">
         <v>3</v>
       </c>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="66">
+      <c r="P33" s="72"/>
+      <c r="Q33" s="71">
         <v>6</v>
       </c>
-      <c r="R33" s="67"/>
-      <c r="S33" s="66">
+      <c r="R33" s="72"/>
+      <c r="S33" s="71">
         <f>Q33-O33</f>
         <v>3</v>
       </c>
-      <c r="T33" s="67"/>
-      <c r="U33" s="66">
+      <c r="T33" s="72"/>
+      <c r="U33" s="71">
         <v>1</v>
       </c>
-      <c r="V33" s="80"/>
-      <c r="W33" s="80"/>
-      <c r="X33" s="67"/>
-      <c r="Y33" s="92" t="str">
+      <c r="V33" s="85"/>
+      <c r="W33" s="85"/>
+      <c r="X33" s="72"/>
+      <c r="Y33" s="100" t="str">
         <f>CONCATENATE("(", B32, " &lt;&lt; ", TEXT(S33, "00"), ") &amp; ", POWER(2, Q33) * (POWER(2, U33) - 1),)</f>
         <v>(e &lt;&lt; 03) &amp; 64</v>
       </c>
-      <c r="Z33" s="93"/>
-      <c r="AA33" s="93"/>
-      <c r="AB33" s="93"/>
-      <c r="AC33" s="93"/>
-      <c r="AD33" s="93"/>
-      <c r="AE33" s="93"/>
-      <c r="AF33" s="93"/>
-      <c r="AG33" s="93"/>
-      <c r="AH33" s="93"/>
-      <c r="AI33" s="94"/>
-      <c r="AJ33" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK33" s="80"/>
-      <c r="AL33" s="80"/>
-      <c r="AM33" s="80"/>
-      <c r="AN33" s="80"/>
-      <c r="AO33" s="80"/>
-      <c r="AP33" s="80"/>
-      <c r="AQ33" s="80"/>
-      <c r="AR33" s="80"/>
-      <c r="AS33" s="80"/>
-      <c r="AT33" s="67"/>
+      <c r="Z33" s="101"/>
+      <c r="AA33" s="101"/>
+      <c r="AB33" s="101"/>
+      <c r="AC33" s="101"/>
+      <c r="AD33" s="101"/>
+      <c r="AE33" s="101"/>
+      <c r="AF33" s="101"/>
+      <c r="AG33" s="101"/>
+      <c r="AH33" s="101"/>
+      <c r="AI33" s="102"/>
+      <c r="AJ33" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK33" s="85"/>
+      <c r="AL33" s="85"/>
+      <c r="AM33" s="85"/>
+      <c r="AN33" s="85"/>
+      <c r="AO33" s="85"/>
+      <c r="AP33" s="85"/>
+      <c r="AQ33" s="85"/>
+      <c r="AR33" s="85"/>
+      <c r="AS33" s="85"/>
+      <c r="AT33" s="72"/>
     </row>
     <row r="34" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
@@ -2748,92 +2811,92 @@
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
       <c r="K34" s="27"/>
-      <c r="M34" s="76" t="s">
+      <c r="M34" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="N34" s="77"/>
-      <c r="O34" s="66">
+      <c r="N34" s="82"/>
+      <c r="O34" s="71">
         <v>4</v>
       </c>
-      <c r="P34" s="67"/>
-      <c r="Q34" s="66">
+      <c r="P34" s="72"/>
+      <c r="Q34" s="71">
         <v>5</v>
       </c>
-      <c r="R34" s="67"/>
-      <c r="S34" s="66">
+      <c r="R34" s="72"/>
+      <c r="S34" s="71">
         <f>Q34-O34</f>
         <v>1</v>
       </c>
-      <c r="T34" s="67"/>
-      <c r="U34" s="66">
+      <c r="T34" s="72"/>
+      <c r="U34" s="71">
         <v>1</v>
       </c>
-      <c r="V34" s="80"/>
-      <c r="W34" s="80"/>
-      <c r="X34" s="67"/>
-      <c r="Y34" s="92" t="str">
+      <c r="V34" s="85"/>
+      <c r="W34" s="85"/>
+      <c r="X34" s="72"/>
+      <c r="Y34" s="100" t="str">
         <f>CONCATENATE("(", B34, " &lt;&lt; ", TEXT(S34, "00"), ") &amp; ", POWER(2, Q34) * (POWER(2, U34) - 1),)</f>
         <v>(f &lt;&lt; 01) &amp; 32</v>
       </c>
-      <c r="Z34" s="93"/>
-      <c r="AA34" s="93"/>
-      <c r="AB34" s="93"/>
-      <c r="AC34" s="93"/>
-      <c r="AD34" s="93"/>
-      <c r="AE34" s="93"/>
-      <c r="AF34" s="93"/>
-      <c r="AG34" s="93"/>
-      <c r="AH34" s="93"/>
-      <c r="AI34" s="94"/>
-      <c r="AJ34" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK34" s="80"/>
-      <c r="AL34" s="80"/>
-      <c r="AM34" s="80"/>
-      <c r="AN34" s="80"/>
-      <c r="AO34" s="80"/>
-      <c r="AP34" s="80"/>
-      <c r="AQ34" s="80"/>
-      <c r="AR34" s="80"/>
-      <c r="AS34" s="80"/>
-      <c r="AT34" s="67"/>
+      <c r="Z34" s="101"/>
+      <c r="AA34" s="101"/>
+      <c r="AB34" s="101"/>
+      <c r="AC34" s="101"/>
+      <c r="AD34" s="101"/>
+      <c r="AE34" s="101"/>
+      <c r="AF34" s="101"/>
+      <c r="AG34" s="101"/>
+      <c r="AH34" s="101"/>
+      <c r="AI34" s="102"/>
+      <c r="AJ34" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK34" s="85"/>
+      <c r="AL34" s="85"/>
+      <c r="AM34" s="85"/>
+      <c r="AN34" s="85"/>
+      <c r="AO34" s="85"/>
+      <c r="AP34" s="85"/>
+      <c r="AQ34" s="85"/>
+      <c r="AR34" s="85"/>
+      <c r="AS34" s="85"/>
+      <c r="AT34" s="72"/>
     </row>
     <row r="35" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M35" s="76"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="67"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="67"/>
-      <c r="U35" s="66"/>
-      <c r="V35" s="80"/>
-      <c r="W35" s="80"/>
-      <c r="X35" s="67"/>
-      <c r="Y35" s="92"/>
-      <c r="Z35" s="93"/>
-      <c r="AA35" s="93"/>
-      <c r="AB35" s="93"/>
-      <c r="AC35" s="93"/>
-      <c r="AD35" s="93"/>
-      <c r="AE35" s="93"/>
-      <c r="AF35" s="93"/>
-      <c r="AG35" s="93"/>
-      <c r="AH35" s="93"/>
-      <c r="AI35" s="94"/>
-      <c r="AJ35" s="66"/>
-      <c r="AK35" s="80"/>
-      <c r="AL35" s="80"/>
-      <c r="AM35" s="80"/>
-      <c r="AN35" s="80"/>
-      <c r="AO35" s="80"/>
-      <c r="AP35" s="80"/>
-      <c r="AQ35" s="80"/>
-      <c r="AR35" s="80"/>
-      <c r="AS35" s="80"/>
-      <c r="AT35" s="67"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="82"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="71"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="71"/>
+      <c r="V35" s="85"/>
+      <c r="W35" s="85"/>
+      <c r="X35" s="72"/>
+      <c r="Y35" s="100"/>
+      <c r="Z35" s="101"/>
+      <c r="AA35" s="101"/>
+      <c r="AB35" s="101"/>
+      <c r="AC35" s="101"/>
+      <c r="AD35" s="101"/>
+      <c r="AE35" s="101"/>
+      <c r="AF35" s="101"/>
+      <c r="AG35" s="101"/>
+      <c r="AH35" s="101"/>
+      <c r="AI35" s="102"/>
+      <c r="AJ35" s="71"/>
+      <c r="AK35" s="85"/>
+      <c r="AL35" s="85"/>
+      <c r="AM35" s="85"/>
+      <c r="AN35" s="85"/>
+      <c r="AO35" s="85"/>
+      <c r="AP35" s="85"/>
+      <c r="AQ35" s="85"/>
+      <c r="AR35" s="85"/>
+      <c r="AS35" s="85"/>
+      <c r="AT35" s="72"/>
     </row>
     <row r="36" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
@@ -2855,92 +2918,92 @@
       <c r="I36" s="24"/>
       <c r="J36" s="24"/>
       <c r="K36" s="27"/>
-      <c r="M36" s="76" t="s">
+      <c r="M36" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="N36" s="77"/>
-      <c r="O36" s="66">
+      <c r="N36" s="82"/>
+      <c r="O36" s="71">
         <v>4</v>
       </c>
-      <c r="P36" s="67"/>
-      <c r="Q36" s="66">
+      <c r="P36" s="72"/>
+      <c r="Q36" s="71">
         <v>1</v>
       </c>
-      <c r="R36" s="67"/>
-      <c r="S36" s="66">
+      <c r="R36" s="72"/>
+      <c r="S36" s="71">
         <f>Q36-O36</f>
         <v>-3</v>
       </c>
-      <c r="T36" s="67"/>
-      <c r="U36" s="66">
+      <c r="T36" s="72"/>
+      <c r="U36" s="71">
         <v>4</v>
       </c>
-      <c r="V36" s="80"/>
-      <c r="W36" s="80"/>
-      <c r="X36" s="67"/>
-      <c r="Y36" s="92" t="str">
+      <c r="V36" s="85"/>
+      <c r="W36" s="85"/>
+      <c r="X36" s="72"/>
+      <c r="Y36" s="100" t="str">
         <f t="shared" si="0"/>
         <v>(g &lt;&lt; -03) &amp; 30</v>
       </c>
-      <c r="Z36" s="93"/>
-      <c r="AA36" s="93"/>
-      <c r="AB36" s="93"/>
-      <c r="AC36" s="93"/>
-      <c r="AD36" s="93"/>
-      <c r="AE36" s="93"/>
-      <c r="AF36" s="93"/>
-      <c r="AG36" s="93"/>
-      <c r="AH36" s="93"/>
-      <c r="AI36" s="94"/>
-      <c r="AJ36" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK36" s="80"/>
-      <c r="AL36" s="80"/>
-      <c r="AM36" s="80"/>
-      <c r="AN36" s="80"/>
-      <c r="AO36" s="80"/>
-      <c r="AP36" s="80"/>
-      <c r="AQ36" s="80"/>
-      <c r="AR36" s="80"/>
-      <c r="AS36" s="80"/>
-      <c r="AT36" s="67"/>
+      <c r="Z36" s="101"/>
+      <c r="AA36" s="101"/>
+      <c r="AB36" s="101"/>
+      <c r="AC36" s="101"/>
+      <c r="AD36" s="101"/>
+      <c r="AE36" s="101"/>
+      <c r="AF36" s="101"/>
+      <c r="AG36" s="101"/>
+      <c r="AH36" s="101"/>
+      <c r="AI36" s="102"/>
+      <c r="AJ36" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK36" s="85"/>
+      <c r="AL36" s="85"/>
+      <c r="AM36" s="85"/>
+      <c r="AN36" s="85"/>
+      <c r="AO36" s="85"/>
+      <c r="AP36" s="85"/>
+      <c r="AQ36" s="85"/>
+      <c r="AR36" s="85"/>
+      <c r="AS36" s="85"/>
+      <c r="AT36" s="72"/>
     </row>
     <row r="37" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M37" s="76"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="67"/>
-      <c r="Q37" s="66"/>
-      <c r="R37" s="67"/>
-      <c r="S37" s="66"/>
-      <c r="T37" s="67"/>
-      <c r="U37" s="66"/>
-      <c r="V37" s="80"/>
-      <c r="W37" s="80"/>
-      <c r="X37" s="67"/>
-      <c r="Y37" s="92"/>
-      <c r="Z37" s="93"/>
-      <c r="AA37" s="93"/>
-      <c r="AB37" s="93"/>
-      <c r="AC37" s="93"/>
-      <c r="AD37" s="93"/>
-      <c r="AE37" s="93"/>
-      <c r="AF37" s="93"/>
-      <c r="AG37" s="93"/>
-      <c r="AH37" s="93"/>
-      <c r="AI37" s="94"/>
-      <c r="AJ37" s="66"/>
-      <c r="AK37" s="80"/>
-      <c r="AL37" s="80"/>
-      <c r="AM37" s="80"/>
-      <c r="AN37" s="80"/>
-      <c r="AO37" s="80"/>
-      <c r="AP37" s="80"/>
-      <c r="AQ37" s="80"/>
-      <c r="AR37" s="80"/>
-      <c r="AS37" s="80"/>
-      <c r="AT37" s="67"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="72"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="72"/>
+      <c r="U37" s="71"/>
+      <c r="V37" s="85"/>
+      <c r="W37" s="85"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="100"/>
+      <c r="Z37" s="101"/>
+      <c r="AA37" s="101"/>
+      <c r="AB37" s="101"/>
+      <c r="AC37" s="101"/>
+      <c r="AD37" s="101"/>
+      <c r="AE37" s="101"/>
+      <c r="AF37" s="101"/>
+      <c r="AG37" s="101"/>
+      <c r="AH37" s="101"/>
+      <c r="AI37" s="102"/>
+      <c r="AJ37" s="71"/>
+      <c r="AK37" s="85"/>
+      <c r="AL37" s="85"/>
+      <c r="AM37" s="85"/>
+      <c r="AN37" s="85"/>
+      <c r="AO37" s="85"/>
+      <c r="AP37" s="85"/>
+      <c r="AQ37" s="85"/>
+      <c r="AR37" s="85"/>
+      <c r="AS37" s="85"/>
+      <c r="AT37" s="72"/>
     </row>
     <row r="38" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
@@ -2956,92 +3019,92 @@
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
       <c r="K38" s="27"/>
-      <c r="M38" s="76" t="s">
+      <c r="M38" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="N38" s="77"/>
-      <c r="O38" s="66">
+      <c r="N38" s="82"/>
+      <c r="O38" s="71">
         <v>7</v>
       </c>
-      <c r="P38" s="67"/>
-      <c r="Q38" s="66">
+      <c r="P38" s="72"/>
+      <c r="Q38" s="71">
         <v>0</v>
       </c>
-      <c r="R38" s="67"/>
-      <c r="S38" s="66">
+      <c r="R38" s="72"/>
+      <c r="S38" s="71">
         <f>Q38-O38</f>
         <v>-7</v>
       </c>
-      <c r="T38" s="67"/>
-      <c r="U38" s="66">
+      <c r="T38" s="72"/>
+      <c r="U38" s="71">
         <v>1</v>
       </c>
-      <c r="V38" s="80"/>
-      <c r="W38" s="80"/>
-      <c r="X38" s="67"/>
-      <c r="Y38" s="92" t="str">
+      <c r="V38" s="85"/>
+      <c r="W38" s="85"/>
+      <c r="X38" s="72"/>
+      <c r="Y38" s="100" t="str">
         <f t="shared" si="0"/>
         <v>(h &lt;&lt; -07) &amp; 1</v>
       </c>
-      <c r="Z38" s="93"/>
-      <c r="AA38" s="93"/>
-      <c r="AB38" s="93"/>
-      <c r="AC38" s="93"/>
-      <c r="AD38" s="93"/>
-      <c r="AE38" s="93"/>
-      <c r="AF38" s="93"/>
-      <c r="AG38" s="93"/>
-      <c r="AH38" s="93"/>
-      <c r="AI38" s="94"/>
-      <c r="AJ38" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK38" s="80"/>
-      <c r="AL38" s="80"/>
-      <c r="AM38" s="80"/>
-      <c r="AN38" s="80"/>
-      <c r="AO38" s="80"/>
-      <c r="AP38" s="80"/>
-      <c r="AQ38" s="80"/>
-      <c r="AR38" s="80"/>
-      <c r="AS38" s="80"/>
-      <c r="AT38" s="67"/>
+      <c r="Z38" s="101"/>
+      <c r="AA38" s="101"/>
+      <c r="AB38" s="101"/>
+      <c r="AC38" s="101"/>
+      <c r="AD38" s="101"/>
+      <c r="AE38" s="101"/>
+      <c r="AF38" s="101"/>
+      <c r="AG38" s="101"/>
+      <c r="AH38" s="101"/>
+      <c r="AI38" s="102"/>
+      <c r="AJ38" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK38" s="85"/>
+      <c r="AL38" s="85"/>
+      <c r="AM38" s="85"/>
+      <c r="AN38" s="85"/>
+      <c r="AO38" s="85"/>
+      <c r="AP38" s="85"/>
+      <c r="AQ38" s="85"/>
+      <c r="AR38" s="85"/>
+      <c r="AS38" s="85"/>
+      <c r="AT38" s="72"/>
     </row>
     <row r="39" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M39" s="76"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="67"/>
-      <c r="Q39" s="66"/>
-      <c r="R39" s="67"/>
-      <c r="S39" s="66"/>
-      <c r="T39" s="67"/>
-      <c r="U39" s="66"/>
-      <c r="V39" s="80"/>
-      <c r="W39" s="80"/>
-      <c r="X39" s="67"/>
-      <c r="Y39" s="92"/>
-      <c r="Z39" s="93"/>
-      <c r="AA39" s="93"/>
-      <c r="AB39" s="93"/>
-      <c r="AC39" s="93"/>
-      <c r="AD39" s="93"/>
-      <c r="AE39" s="93"/>
-      <c r="AF39" s="93"/>
-      <c r="AG39" s="93"/>
-      <c r="AH39" s="93"/>
-      <c r="AI39" s="94"/>
-      <c r="AJ39" s="66"/>
-      <c r="AK39" s="80"/>
-      <c r="AL39" s="80"/>
-      <c r="AM39" s="80"/>
-      <c r="AN39" s="80"/>
-      <c r="AO39" s="80"/>
-      <c r="AP39" s="80"/>
-      <c r="AQ39" s="80"/>
-      <c r="AR39" s="80"/>
-      <c r="AS39" s="80"/>
-      <c r="AT39" s="67"/>
+      <c r="M39" s="81"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="71"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="71"/>
+      <c r="T39" s="72"/>
+      <c r="U39" s="71"/>
+      <c r="V39" s="85"/>
+      <c r="W39" s="85"/>
+      <c r="X39" s="72"/>
+      <c r="Y39" s="100"/>
+      <c r="Z39" s="101"/>
+      <c r="AA39" s="101"/>
+      <c r="AB39" s="101"/>
+      <c r="AC39" s="101"/>
+      <c r="AD39" s="101"/>
+      <c r="AE39" s="101"/>
+      <c r="AF39" s="101"/>
+      <c r="AG39" s="101"/>
+      <c r="AH39" s="101"/>
+      <c r="AI39" s="102"/>
+      <c r="AJ39" s="71"/>
+      <c r="AK39" s="85"/>
+      <c r="AL39" s="85"/>
+      <c r="AM39" s="85"/>
+      <c r="AN39" s="85"/>
+      <c r="AO39" s="85"/>
+      <c r="AP39" s="85"/>
+      <c r="AQ39" s="85"/>
+      <c r="AR39" s="85"/>
+      <c r="AS39" s="85"/>
+      <c r="AT39" s="72"/>
     </row>
     <row r="40" spans="2:46" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
@@ -3071,111 +3134,282 @@
       <c r="K40" s="42">
         <v>16</v>
       </c>
-      <c r="M40" s="76" t="s">
+      <c r="M40" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="N40" s="77"/>
-      <c r="O40" s="66">
+      <c r="N40" s="82"/>
+      <c r="O40" s="71">
         <v>4</v>
       </c>
-      <c r="P40" s="67"/>
-      <c r="Q40" s="66">
+      <c r="P40" s="72"/>
+      <c r="Q40" s="71">
         <v>13</v>
       </c>
-      <c r="R40" s="67"/>
-      <c r="S40" s="66">
+      <c r="R40" s="72"/>
+      <c r="S40" s="71">
         <f>Q40-O40</f>
         <v>9</v>
       </c>
-      <c r="T40" s="67"/>
-      <c r="U40" s="66">
+      <c r="T40" s="72"/>
+      <c r="U40" s="71">
         <v>4</v>
       </c>
-      <c r="V40" s="80"/>
-      <c r="W40" s="80"/>
-      <c r="X40" s="67"/>
-      <c r="Y40" s="92" t="str">
+      <c r="V40" s="85"/>
+      <c r="W40" s="85"/>
+      <c r="X40" s="72"/>
+      <c r="Y40" s="100" t="str">
         <f t="shared" si="0"/>
         <v>(x &lt;&lt; 09) &amp; 122880</v>
       </c>
-      <c r="Z40" s="93"/>
-      <c r="AA40" s="93"/>
-      <c r="AB40" s="93"/>
-      <c r="AC40" s="93"/>
-      <c r="AD40" s="93"/>
-      <c r="AE40" s="93"/>
-      <c r="AF40" s="93"/>
-      <c r="AG40" s="93"/>
-      <c r="AH40" s="93"/>
-      <c r="AI40" s="94"/>
-      <c r="AJ40" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK40" s="80"/>
-      <c r="AL40" s="80"/>
-      <c r="AM40" s="80"/>
-      <c r="AN40" s="80"/>
-      <c r="AO40" s="80"/>
-      <c r="AP40" s="80"/>
-      <c r="AQ40" s="80"/>
-      <c r="AR40" s="80"/>
-      <c r="AS40" s="80"/>
-      <c r="AT40" s="67"/>
+      <c r="Z40" s="101"/>
+      <c r="AA40" s="101"/>
+      <c r="AB40" s="101"/>
+      <c r="AC40" s="101"/>
+      <c r="AD40" s="101"/>
+      <c r="AE40" s="101"/>
+      <c r="AF40" s="101"/>
+      <c r="AG40" s="101"/>
+      <c r="AH40" s="101"/>
+      <c r="AI40" s="102"/>
+      <c r="AJ40" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK40" s="85"/>
+      <c r="AL40" s="85"/>
+      <c r="AM40" s="85"/>
+      <c r="AN40" s="85"/>
+      <c r="AO40" s="85"/>
+      <c r="AP40" s="85"/>
+      <c r="AQ40" s="85"/>
+      <c r="AR40" s="85"/>
+      <c r="AS40" s="85"/>
+      <c r="AT40" s="72"/>
     </row>
     <row r="41" spans="2:46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M41" s="68" t="s">
+      <c r="M41" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="N41" s="69"/>
-      <c r="O41" s="70">
+      <c r="N41" s="74"/>
+      <c r="O41" s="75">
         <v>0</v>
       </c>
-      <c r="P41" s="71"/>
-      <c r="Q41" s="70">
+      <c r="P41" s="76"/>
+      <c r="Q41" s="75">
         <v>7</v>
       </c>
-      <c r="R41" s="71"/>
-      <c r="S41" s="70">
+      <c r="R41" s="76"/>
+      <c r="S41" s="75">
         <f>Q41-O41</f>
         <v>7</v>
       </c>
-      <c r="T41" s="71"/>
-      <c r="U41" s="70">
+      <c r="T41" s="76"/>
+      <c r="U41" s="75">
         <v>4</v>
       </c>
-      <c r="V41" s="85"/>
-      <c r="W41" s="85"/>
-      <c r="X41" s="71"/>
-      <c r="Y41" s="95" t="str">
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
+      <c r="X41" s="76"/>
+      <c r="Y41" s="103" t="str">
         <f>CONCATENATE("(", B40, " &lt;&lt; ", TEXT(S41, "00"), ") &amp; ", POWER(2, Q41) * (POWER(2, U41) - 1),)</f>
         <v>(x &lt;&lt; 07) &amp; 1920</v>
       </c>
-      <c r="Z41" s="96"/>
-      <c r="AA41" s="96"/>
-      <c r="AB41" s="96"/>
-      <c r="AC41" s="96"/>
-      <c r="AD41" s="96"/>
-      <c r="AE41" s="96"/>
-      <c r="AF41" s="96"/>
-      <c r="AG41" s="96"/>
-      <c r="AH41" s="96"/>
-      <c r="AI41" s="97"/>
-      <c r="AJ41" s="70" t="s">
+      <c r="Z41" s="104"/>
+      <c r="AA41" s="104"/>
+      <c r="AB41" s="104"/>
+      <c r="AC41" s="104"/>
+      <c r="AD41" s="104"/>
+      <c r="AE41" s="104"/>
+      <c r="AF41" s="104"/>
+      <c r="AG41" s="104"/>
+      <c r="AH41" s="104"/>
+      <c r="AI41" s="105"/>
+      <c r="AJ41" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK41" s="90"/>
+      <c r="AL41" s="90"/>
+      <c r="AM41" s="90"/>
+      <c r="AN41" s="90"/>
+      <c r="AO41" s="90"/>
+      <c r="AP41" s="90"/>
+      <c r="AQ41" s="90"/>
+      <c r="AR41" s="90"/>
+      <c r="AS41" s="90"/>
+      <c r="AT41" s="76"/>
+    </row>
+    <row r="58" spans="4:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P58" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="AK41" s="85"/>
-      <c r="AL41" s="85"/>
-      <c r="AM41" s="85"/>
-      <c r="AN41" s="85"/>
-      <c r="AO41" s="85"/>
-      <c r="AP41" s="85"/>
-      <c r="AQ41" s="85"/>
-      <c r="AR41" s="85"/>
-      <c r="AS41" s="85"/>
-      <c r="AT41" s="71"/>
+      <c r="Q58" s="70"/>
+      <c r="R58" s="70"/>
+      <c r="S58" s="70"/>
+      <c r="T58" s="70"/>
+      <c r="U58" s="70"/>
+      <c r="V58" s="70"/>
+      <c r="W58" s="70"/>
+    </row>
+    <row r="60" spans="4:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="1">
+        <v>24</v>
+      </c>
+      <c r="S60" s="1">
+        <v>16</v>
+      </c>
+      <c r="AA60" s="1">
+        <v>8</v>
+      </c>
+      <c r="AI60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="66">
+        <v>3</v>
+      </c>
+      <c r="E61" s="66">
+        <v>3</v>
+      </c>
+      <c r="F61" s="66">
+        <v>3</v>
+      </c>
+      <c r="G61" s="66">
+        <v>3</v>
+      </c>
+      <c r="H61" s="66">
+        <v>3</v>
+      </c>
+      <c r="I61" s="66">
+        <v>3</v>
+      </c>
+      <c r="J61" s="66">
+        <v>3</v>
+      </c>
+      <c r="K61" s="66">
+        <v>3</v>
+      </c>
+      <c r="L61" s="67">
+        <v>2</v>
+      </c>
+      <c r="M61" s="67">
+        <v>2</v>
+      </c>
+      <c r="N61" s="67">
+        <v>2</v>
+      </c>
+      <c r="O61" s="67">
+        <v>2</v>
+      </c>
+      <c r="P61" s="67">
+        <v>2</v>
+      </c>
+      <c r="Q61" s="67">
+        <v>2</v>
+      </c>
+      <c r="R61" s="67">
+        <v>2</v>
+      </c>
+      <c r="S61" s="67">
+        <v>2</v>
+      </c>
+      <c r="T61" s="68">
+        <v>1</v>
+      </c>
+      <c r="U61" s="68">
+        <v>1</v>
+      </c>
+      <c r="V61" s="68">
+        <v>1</v>
+      </c>
+      <c r="W61" s="68">
+        <v>1</v>
+      </c>
+      <c r="X61" s="68">
+        <v>1</v>
+      </c>
+      <c r="Y61" s="68">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="68">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="68">
+        <v>1</v>
+      </c>
+      <c r="AB61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AD61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AF61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AG61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AH61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AI61" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="R63" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z63" s="8"/>
+    </row>
+    <row r="64" spans="4:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="R64" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="4:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="4:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="4:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="150">
+  <mergeCells count="151">
     <mergeCell ref="AJ41:AT41"/>
     <mergeCell ref="AJ40:AT40"/>
     <mergeCell ref="AJ33:AT33"/>
@@ -3236,13 +3470,6 @@
     <mergeCell ref="AN5:AN6"/>
     <mergeCell ref="Y23:AI23"/>
     <mergeCell ref="Y24:AI24"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="U25:X25"/>
-    <mergeCell ref="U26:X26"/>
     <mergeCell ref="Q23:R23"/>
     <mergeCell ref="Q35:R35"/>
     <mergeCell ref="S29:T29"/>
@@ -3252,19 +3479,26 @@
     <mergeCell ref="S33:T33"/>
     <mergeCell ref="S34:T34"/>
     <mergeCell ref="S35:T35"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="U27:X27"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="U30:X30"/>
+    <mergeCell ref="U31:X31"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="U25:X25"/>
+    <mergeCell ref="U26:X26"/>
     <mergeCell ref="S36:T36"/>
     <mergeCell ref="S37:T37"/>
     <mergeCell ref="U39:X39"/>
     <mergeCell ref="U40:X40"/>
     <mergeCell ref="U41:X41"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
     <mergeCell ref="S38:T38"/>
     <mergeCell ref="U32:X32"/>
     <mergeCell ref="U33:X33"/>
@@ -3274,22 +3508,17 @@
     <mergeCell ref="U38:X38"/>
     <mergeCell ref="U37:X37"/>
     <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O32:P32"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O26:P26"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q32:R32"/>
     <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="U27:X27"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="U30:X30"/>
-    <mergeCell ref="U31:X31"/>
-    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="M35:N35"/>
     <mergeCell ref="M32:N32"/>
@@ -3302,6 +3531,13 @@
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="O38:P38"/>
     <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="P58:W58"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="M41:N41"/>
     <mergeCell ref="O41:P41"/>
@@ -3325,7 +3561,6 @@
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final changes before a release
- Moved shared shader logic to a separate .cginc file and refactored the double buffering logic
- Refactored the usage of shader keywords and created #defines for double buffering and usage of StructuredBuffer vs. RWStructuredBuffer
- reduced VRAM usage by ~4 times by using byte packing for double buffering
- cleaned up most of the C# source code
</commit_message>
<xml_diff>
--- a/Assets/Docs/LookupTables.xlsx
+++ b/Assets/Docs/LookupTables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Unity\Editor\Shaders\Assets\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Unity\Editor\ShaderLife\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AT67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3510,6 +3510,7 @@
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="U31:X31"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="M35:N35"/>
@@ -3529,7 +3530,6 @@
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="U37:X37"/>
     <mergeCell ref="Q36:R36"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="O31:P31"/>
@@ -3541,11 +3541,6 @@
     <mergeCell ref="Q28:R28"/>
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="U27:X27"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="U30:X30"/>
-    <mergeCell ref="U31:X31"/>
     <mergeCell ref="S39:T39"/>
     <mergeCell ref="S40:T40"/>
     <mergeCell ref="S41:T41"/>
@@ -3565,6 +3560,11 @@
     <mergeCell ref="U35:X35"/>
     <mergeCell ref="U36:X36"/>
     <mergeCell ref="U38:X38"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="U27:X27"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="U30:X30"/>
     <mergeCell ref="Q23:R23"/>
     <mergeCell ref="Q35:R35"/>
     <mergeCell ref="S29:T29"/>
@@ -3640,6 +3640,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="Y33 Y31" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>